<commit_message>
Fixed scripts in ENWIAM Module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENWIAM.xlsx
+++ b/src/test/resources/xls/ENWIAM.xlsx
@@ -4,18 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="3900"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="13296" windowHeight="3900"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
-    <sheet name="IAM005" sheetId="5" r:id="rId2"/>
+    <sheet name="ENWIAM002" sheetId="5" r:id="rId2"/>
+    <sheet name="ENWIAM003" sheetId="7" r:id="rId3"/>
+    <sheet name="ENWIAM004" sheetId="8" r:id="rId4"/>
+    <sheet name="ENWIAM005" sheetId="9" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="54">
   <si>
     <t>TCID</t>
   </si>
@@ -50,13 +53,137 @@
     <t>Jira id</t>
   </si>
   <si>
-    <t>TBD</t>
-  </si>
-  <si>
-    <t>Need to add test case description</t>
-  </si>
-  <si>
     <t>ENWIAM001</t>
+  </si>
+  <si>
+    <t>OPQA-1719||
+OPQA-1676||OPQA-1744||
+OPQA-1760||OPQA-1763
+||OPQA-1766</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that ENW registration screen should be displayed and User should be able to enter email address (required), name (required), and password (required).||Verify that "Sign up" link should be displayed on ENW registration page .||Verify that the user should be able click on "sign up" button after filling the above fields correctly.||Verify that user should get an Email verification Link on the registered Email Id .||Verify that after clicking verification link user should get the message as" Success!You have successfully activated your account. Please sign in."||Verify that after completion of verification process,user should be able to sign into ENW </t>
+  </si>
+  <si>
+    <t>OPQA-1731</t>
+  </si>
+  <si>
+    <t>Verify that email address field should be in standard email ID format .Email address fields should be mandatory.</t>
+  </si>
+  <si>
+    <t>SUFFIX</t>
+  </si>
+  <si>
+    <t>ERROR TEXT</t>
+  </si>
+  <si>
+    <t>@abc.com</t>
+  </si>
+  <si>
+    <t>Please enter no more than 255 characters.</t>
+  </si>
+  <si>
+    <t>Please enter a valid Email Address.</t>
+  </si>
+  <si>
+    <t>OPQA-1741</t>
+  </si>
+  <si>
+    <t>Verify that Passwords should be at least 8 characters,Must contain at least 1 lowercase letter,Must contain at least 1 uppercase letter,Must contain at least 1 number,should have at least one special character and must not be empty.</t>
+  </si>
+  <si>
+    <t>ENWIAM002</t>
+  </si>
+  <si>
+    <t>ENWIAM003</t>
+  </si>
+  <si>
+    <t>PASSWORD</t>
+  </si>
+  <si>
+    <t>STRENGTH</t>
+  </si>
+  <si>
+    <t>TICK MARKS</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Weak</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>Ne</t>
+  </si>
+  <si>
+    <t>Neo3</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>Neon@</t>
+  </si>
+  <si>
+    <t>Neon@123</t>
+  </si>
+  <si>
+    <t>Strong</t>
+  </si>
+  <si>
+    <t>OPQA-1743</t>
+  </si>
+  <si>
+    <t>Verify that first name should be maximum of 50 characters long and these fields should not be empty.</t>
+  </si>
+  <si>
+    <t>Verify that last name should be maximum of 50 characters long and these fields should not be empty.</t>
+  </si>
+  <si>
+    <t>ENWIAM004</t>
+  </si>
+  <si>
+    <t>ENWIAM005</t>
+  </si>
+  <si>
+    <t>OPQA-1755</t>
+  </si>
+  <si>
+    <t>Verify that user should not have a ENW account created if the email address provided on the ENW registration screen already exists in neon identity and a message should be displayed as"Already have an account? and proceed to sign-in"</t>
+  </si>
+  <si>
+    <t>ENWIAM006</t>
+  </si>
+  <si>
+    <t>ENWIAM007</t>
+  </si>
+  <si>
+    <t>Verify that user should not have a ENW account created if the email address provided on the ENW registration screen already exists in STeAM and and a message should be displayed as" email address already exists and proceed to sign-in"</t>
+  </si>
+  <si>
+    <t>OPQA-1747</t>
+  </si>
+  <si>
+    <t>ENWIAM008</t>
+  </si>
+  <si>
+    <t>OPQA-1758</t>
+  </si>
+  <si>
+    <t>Verify that system should remove any leading or trailing spaces of an email address entered by the user before validating it.</t>
+  </si>
+  <si>
+    <t>OPQA-1963||
+OPQA-1964||OPQA-1965||OPQA-1966</t>
+  </si>
+  <si>
+    <t>Verify that "View additional email preferences" should be displayed in the account setting page.||Verify that after clicking "View additional email preferences" user should be redirected to "Intelectual property and Science Page" and should be able to enter email id in email Address field to access your preference center.||Verify that user should receive an email verification mail containing a direct link to "Preference Center" Page, where user can update email preferences for the "Intellectual Property &amp; Science business of Thomson Reuters."||Verify that after updating the preferences ,the system should update the URL that supports the "View additional email preferences" link .</t>
+  </si>
+  <si>
+    <t>ENWIAM009</t>
   </si>
 </sst>
 </file>
@@ -79,7 +206,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -92,8 +219,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -116,6 +249,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -124,13 +268,25 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -428,19 +584,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="70.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.44140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="70.6640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.33203125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -460,20 +616,156 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:5" ht="115.2">
+      <c r="A2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="28.8">
+      <c r="A3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="43.2">
+      <c r="A4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="28.8">
+      <c r="A5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="28.8">
+      <c r="A6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="43.2">
+      <c r="A7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="57.6">
+      <c r="A8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="28.8">
+      <c r="A9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="129.6">
+      <c r="A10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>4</v>
       </c>
     </row>
@@ -485,16 +777,374 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="18.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="3">
+        <v>246</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="3">
+        <v>247</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="3">
+        <v>248</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="2">
+        <v>111</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="2">
+        <v>111</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="amneetsingh72@gmail.com"/>
+    <hyperlink ref="A4" r:id="rId2" display="amneetsinghasr@gmail.com"/>
+    <hyperlink ref="A3" r:id="rId3" display="amneetsingh100@gmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="2">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="2">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A5" r:id="rId1"/>
+    <hyperlink ref="A6" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2">
+        <v>49</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2">
+        <v>50</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="2">
+        <v>51</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -515,7 +1165,7 @@
       <c r="A2" s="2">
         <v>49</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -529,7 +1179,7 @@
       <c r="A3" s="2">
         <v>50</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -543,7 +1193,7 @@
       <c r="A4" s="2">
         <v>51</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -555,6 +1205,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changed ENWIAM excel file.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENWIAM.xlsx
+++ b/src/test/resources/xls/ENWIAM.xlsx
@@ -15,7 +15,6 @@
     <sheet name="ENWIAM016" sheetId="10" r:id="rId6"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -227,9 +226,6 @@
     <t>ENWIAM014</t>
   </si>
   <si>
-    <t>Verify that,an error message should display as "email activation",when User did'nt activate the link in that respective mail after completing the registration process in ENW.||Verify that system should force the users to verify their email address upon sign in to Neon or ENW with STeAM and provide a way for the user to send another email verification to the user's email address.||Verify that,after clicking the button on resend email verification,the Neon or ENW login page should display a message that informs the user as the email has been sent.||Verify that,user should sent to ENW home page after clicking the link in the ENW verification email.||Verify that system should force the users to verify their email address upon sign in to Neon or ENW with STeAM and provide a way for the user to send another email verification to the user's email address.</t>
-  </si>
-  <si>
     <t>ENWIAM015</t>
   </si>
   <si>
@@ -262,6 +258,9 @@
   </si>
   <si>
     <t>Verify that A user signing in to NEON or ENW using STeAM shall be locked out of their account after 10 invalid attempts.</t>
+  </si>
+  <si>
+    <t>Verify that,an error message should display as "email activation",when User did'nt activate the link in that respective mail after completing the registration process in ENW.||Verify that,the system should send an email verification to the correct email address after clicking the button "Resend Activation" on resend email verification page.||Verify that,after clicking the button on resend email verification,the Neon or ENW login page should display a message that informs the user as the email has been sent.||Verify that,user should sent to ENW home page after clicking the link in the ENW verification email.||Verify that system should force the users to verify their email address upon sign in to Neon or ENW with STeAM and provide a way for the user to send another email verification to the user's email address.</t>
   </si>
 </sst>
 </file>
@@ -664,8 +663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -915,15 +914,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="158.4">
+    <row r="15" spans="1:5" ht="144">
       <c r="A15" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>3</v>
@@ -934,13 +933,13 @@
     </row>
     <row r="16" spans="1:5" ht="43.2">
       <c r="A16" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="C16" s="7" t="s">
         <v>69</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>70</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>3</v>
@@ -951,13 +950,13 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="C17" s="7" t="s">
         <v>72</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>73</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>3</v>
@@ -968,13 +967,13 @@
     </row>
     <row r="18" spans="1:5" ht="28.8">
       <c r="A18" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="C18" s="7" t="s">
         <v>76</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>77</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
ENW login linking flows
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENWIAM.xlsx
+++ b/src/test/resources/xls/ENWIAM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="13296" windowHeight="3900"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="3900"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="84">
   <si>
     <t>TCID</t>
   </si>
@@ -261,6 +261,37 @@
   </si>
   <si>
     <t>Verify that,an error message should display as "email activation",when User did'nt activate the link in that respective mail after completing the registration process in ENW.||Verify that,the system should send an email verification to the correct email address after clicking the button "Resend Activation" on resend email verification page.||Verify that,after clicking the button on resend email verification,the Neon or ENW login page should display a message that informs the user as the email has been sent.||Verify that,user should sent to ENW home page after clicking the link in the ENW verification email.||Verify that system should force the users to verify their email address upon sign in to Neon or ENW with STeAM and provide a way for the user to send another email verification to the user's email address.</t>
+  </si>
+  <si>
+    <t>ENWIAM0001</t>
+  </si>
+  <si>
+    <t>OPQA-1862 || OPQA-1863 || OPQA-1864 || OPQA-1867 || OPQA-1869 || OPQA-3644</t>
+  </si>
+  <si>
+    <t>Verify Upon a successful sign-in for the first time on the ENW landing screen using Social account,the user shall be prompted to link existing Neon accounts that have a STeAM account only with the same email address as the authenticated Social account.
+Verify that the user shall be required to have a linked STeAM account before accessing ENW .
+Verify In order to link or merge the New Social account with an existing Neon account, the user shall be forced to authenticate the existing Neon account.
+Verify that after sign in to ENW landing screen using Facebook, users who already has Steam account with the same email address are prompted to link their Steam account first as precedence with the newly created Facebook account. 
+Verfiy that the user shall be prompted to link the STeAM account by providing a correct password, When linking a STeAM with matching email.
+From ENW,Verify that the system shall only present a single link/merge to a user for each sign in , when a merge includes 3 potential Neon accounts</t>
+  </si>
+  <si>
+    <t>ENWIAM0002</t>
+  </si>
+  <si>
+    <t>OPQA-2373 || OPQA-2375 || OPQA-2377 || OPQA-2379 || OPQA-2381 || OPQA-2383 || OPQA-2385 || OPQA-2404 || OPQA-2405</t>
+  </si>
+  <si>
+    <t>Verify that,After clicking "Sign Up with Facebook" button on ENW landing screen and user does not have STeAM account exists with this email,then an overlay should display as "Thanks for Signing into EndNote Online via Facebook " .
+Verify that,after getting "Thanks for Signing into EndNote Online via Facebook " overlay, click "Yes, I have an account" button to get "Link Accounts" overlay and enter the valid STeAM authenticates credentials on "Link Account" overlay
+Verify that,STeAM should authenticates credentials after entering existing Endnote Online account to link to your FaceBook account and clicking "Done" button on "Link Accounts" overlay.
+Verify that,after providing correct credentials of an existing STeAM account, the system shall link or merge the STeAM account to the newly registered FaceBook account according to the account merge logic.
+Verify that,After clicking "Sign Up with LinkedIn" button on ENW landing screen and user does not have STeAM account exists with this email,then an overlay should display as "Thanks for Signing into EndNote Online via LinkedIn".
+Verify that,after getting "Thanks for Signing into EndNote Online via LinkedIn " overlay, click "Yes, I have an account" button to get "Link Accounts" overlay and enter the valid STeAM authenticates credentials on "Link Account" overlay.
+Verify that,STeAM should authenticates credentials after entering existing Endnote Online account to link to your LinkedIn account and clicking "Done" button on "Link Accounts" overlay.
+Verify that user should be prompted to provide a STeAM account email and password,if If the user clicks the button to link an existing STeAM account with a non-matching email address.
+"Verify that the system should link or merge the STeAM account to the newly registered social account,after providing the correct credentials of an existing STeAM account.</t>
   </si>
 </sst>
 </file>
@@ -661,19 +692,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="70.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="70.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -693,7 +724,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="115.2">
+    <row r="2" spans="1:5" ht="135">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -710,7 +741,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="28.8">
+    <row r="3" spans="1:5" ht="30">
       <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
@@ -727,7 +758,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="43.2">
+    <row r="4" spans="1:5" ht="60">
       <c r="A4" s="2" t="s">
         <v>24</v>
       </c>
@@ -744,7 +775,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="28.8">
+    <row r="5" spans="1:5" ht="30">
       <c r="A5" s="2" t="s">
         <v>40</v>
       </c>
@@ -761,7 +792,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="28.8">
+    <row r="6" spans="1:5" ht="30">
       <c r="A6" s="2" t="s">
         <v>41</v>
       </c>
@@ -778,7 +809,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="43.2">
+    <row r="7" spans="1:5" ht="60">
       <c r="A7" s="2" t="s">
         <v>44</v>
       </c>
@@ -795,7 +826,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="57.6">
+    <row r="8" spans="1:5" ht="60">
       <c r="A8" s="2" t="s">
         <v>45</v>
       </c>
@@ -812,7 +843,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="28.8">
+    <row r="9" spans="1:5" ht="30">
       <c r="A9" s="2" t="s">
         <v>48</v>
       </c>
@@ -829,7 +860,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="129.6">
+    <row r="10" spans="1:5" ht="150">
       <c r="A10" s="2" t="s">
         <v>53</v>
       </c>
@@ -846,7 +877,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="100.8">
+    <row r="11" spans="1:5" ht="105">
       <c r="A11" s="2" t="s">
         <v>54</v>
       </c>
@@ -897,7 +928,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="201.6">
+    <row r="14" spans="1:5" ht="225">
       <c r="A14" s="2" t="s">
         <v>63</v>
       </c>
@@ -914,7 +945,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="144">
+    <row r="15" spans="1:5" ht="165">
       <c r="A15" s="2" t="s">
         <v>66</v>
       </c>
@@ -931,7 +962,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="43.2">
+    <row r="16" spans="1:5" ht="45">
       <c r="A16" s="2" t="s">
         <v>67</v>
       </c>
@@ -965,7 +996,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="28.8">
+    <row r="18" spans="1:5" ht="30">
       <c r="A18" s="2" t="s">
         <v>74</v>
       </c>
@@ -979,6 +1010,40 @@
         <v>3</v>
       </c>
       <c r="E18" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="255">
+      <c r="A19" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="330">
+      <c r="A20" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="6" t="s">
         <v>4</v>
       </c>
     </row>
@@ -996,13 +1061,13 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1136,12 +1201,12 @@
       <selection sqref="A1:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1281,7 +1346,7 @@
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
@@ -1352,12 +1417,12 @@
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1429,10 +1494,10 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">

</xml_diff>

<commit_message>
Modified and Added new test scripts in ENWIAM Module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENWIAM.xlsx
+++ b/src/test/resources/xls/ENWIAM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="3900"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="13296" windowHeight="3900"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="90">
   <si>
     <t>TCID</t>
   </si>
@@ -292,6 +292,24 @@
 Verify that,STeAM should authenticates credentials after entering existing Endnote Online account to link to your LinkedIn account and clicking "Done" button on "Link Accounts" overlay.
 Verify that user should be prompted to provide a STeAM account email and password,if If the user clicks the button to link an existing STeAM account with a non-matching email address.
 "Verify that the system should link or merge the STeAM account to the newly registered social account,after providing the correct credentials of an existing STeAM account.</t>
+  </si>
+  <si>
+    <t>ENWIAM018</t>
+  </si>
+  <si>
+    <t>OPQA-3808</t>
+  </si>
+  <si>
+    <t>Verify that 'Receive email notifications for likes, comments and other activity.' checkbox should work correctly in account setting page.</t>
+  </si>
+  <si>
+    <t>ENWIAM019</t>
+  </si>
+  <si>
+    <t>OPQA-1916</t>
+  </si>
+  <si>
+    <t>The system should send the user through the Neon/ENW password reset workflow when a user clicks 'Change Password' on the Neon/ENW Account settings page .</t>
   </si>
 </sst>
 </file>
@@ -692,19 +710,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="70.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.44140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="70.6640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.33203125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -724,7 +742,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="135">
+    <row r="2" spans="1:5" ht="115.2">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -741,7 +759,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30">
+    <row r="3" spans="1:5" ht="28.8">
       <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
@@ -758,7 +776,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="60">
+    <row r="4" spans="1:5" ht="43.2">
       <c r="A4" s="2" t="s">
         <v>24</v>
       </c>
@@ -775,7 +793,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30">
+    <row r="5" spans="1:5" ht="28.8">
       <c r="A5" s="2" t="s">
         <v>40</v>
       </c>
@@ -792,7 +810,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30">
+    <row r="6" spans="1:5" ht="28.8">
       <c r="A6" s="2" t="s">
         <v>41</v>
       </c>
@@ -809,7 +827,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="60">
+    <row r="7" spans="1:5" ht="43.2">
       <c r="A7" s="2" t="s">
         <v>44</v>
       </c>
@@ -826,7 +844,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="60">
+    <row r="8" spans="1:5" ht="57.6">
       <c r="A8" s="2" t="s">
         <v>45</v>
       </c>
@@ -843,7 +861,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="30">
+    <row r="9" spans="1:5" ht="28.8">
       <c r="A9" s="2" t="s">
         <v>48</v>
       </c>
@@ -860,7 +878,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="150">
+    <row r="10" spans="1:5" ht="129.6">
       <c r="A10" s="2" t="s">
         <v>53</v>
       </c>
@@ -877,7 +895,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="105">
+    <row r="11" spans="1:5" ht="100.8">
       <c r="A11" s="2" t="s">
         <v>54</v>
       </c>
@@ -928,7 +946,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="225">
+    <row r="14" spans="1:5" ht="201.6">
       <c r="A14" s="2" t="s">
         <v>63</v>
       </c>
@@ -945,7 +963,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="165">
+    <row r="15" spans="1:5" ht="144">
       <c r="A15" s="2" t="s">
         <v>66</v>
       </c>
@@ -962,7 +980,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="45">
+    <row r="16" spans="1:5" ht="43.2">
       <c r="A16" s="2" t="s">
         <v>67</v>
       </c>
@@ -996,7 +1014,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="30">
+    <row r="18" spans="1:5" ht="28.8">
       <c r="A18" s="2" t="s">
         <v>74</v>
       </c>
@@ -1013,7 +1031,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="255">
+    <row r="19" spans="1:5" ht="216">
       <c r="A19" s="2" t="s">
         <v>78</v>
       </c>
@@ -1030,7 +1048,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="330">
+    <row r="20" spans="1:5" ht="273.60000000000002">
       <c r="A20" s="2" t="s">
         <v>81</v>
       </c>
@@ -1044,6 +1062,40 @@
         <v>3</v>
       </c>
       <c r="E20" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="28.8">
+      <c r="A21" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="28.8">
+      <c r="A22" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1061,13 +1113,13 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1201,12 +1253,12 @@
       <selection sqref="A1:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1346,7 +1398,7 @@
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
@@ -1417,12 +1469,12 @@
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1494,10 +1546,10 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">

</xml_diff>

<commit_message>
Modified ENW linking flows
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENWIAM.xlsx
+++ b/src/test/resources/xls/ENWIAM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="13296" windowHeight="3900"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="3900"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -269,31 +269,12 @@
     <t>OPQA-1862 || OPQA-1863 || OPQA-1864 || OPQA-1867 || OPQA-1869 || OPQA-3644</t>
   </si>
   <si>
-    <t>Verify Upon a successful sign-in for the first time on the ENW landing screen using Social account,the user shall be prompted to link existing Neon accounts that have a STeAM account only with the same email address as the authenticated Social account.
-Verify that the user shall be required to have a linked STeAM account before accessing ENW .
-Verify In order to link or merge the New Social account with an existing Neon account, the user shall be forced to authenticate the existing Neon account.
-Verify that after sign in to ENW landing screen using Facebook, users who already has Steam account with the same email address are prompted to link their Steam account first as precedence with the newly created Facebook account. 
-Verfiy that the user shall be prompted to link the STeAM account by providing a correct password, When linking a STeAM with matching email.
-From ENW,Verify that the system shall only present a single link/merge to a user for each sign in , when a merge includes 3 potential Neon accounts</t>
-  </si>
-  <si>
     <t>ENWIAM0002</t>
   </si>
   <si>
     <t>OPQA-2373 || OPQA-2375 || OPQA-2377 || OPQA-2379 || OPQA-2381 || OPQA-2383 || OPQA-2385 || OPQA-2404 || OPQA-2405</t>
   </si>
   <si>
-    <t>Verify that,After clicking "Sign Up with Facebook" button on ENW landing screen and user does not have STeAM account exists with this email,then an overlay should display as "Thanks for Signing into EndNote Online via Facebook " .
-Verify that,after getting "Thanks for Signing into EndNote Online via Facebook " overlay, click "Yes, I have an account" button to get "Link Accounts" overlay and enter the valid STeAM authenticates credentials on "Link Account" overlay
-Verify that,STeAM should authenticates credentials after entering existing Endnote Online account to link to your FaceBook account and clicking "Done" button on "Link Accounts" overlay.
-Verify that,after providing correct credentials of an existing STeAM account, the system shall link or merge the STeAM account to the newly registered FaceBook account according to the account merge logic.
-Verify that,After clicking "Sign Up with LinkedIn" button on ENW landing screen and user does not have STeAM account exists with this email,then an overlay should display as "Thanks for Signing into EndNote Online via LinkedIn".
-Verify that,after getting "Thanks for Signing into EndNote Online via LinkedIn " overlay, click "Yes, I have an account" button to get "Link Accounts" overlay and enter the valid STeAM authenticates credentials on "Link Account" overlay.
-Verify that,STeAM should authenticates credentials after entering existing Endnote Online account to link to your LinkedIn account and clicking "Done" button on "Link Accounts" overlay.
-Verify that user should be prompted to provide a STeAM account email and password,if If the user clicks the button to link an existing STeAM account with a non-matching email address.
-"Verify that the system should link or merge the STeAM account to the newly registered social account,after providing the correct credentials of an existing STeAM account.</t>
-  </si>
-  <si>
     <t>ENWIAM018</t>
   </si>
   <si>
@@ -310,13 +291,20 @@
   </si>
   <si>
     <t>The system should send the user through the Neon/ENW password reset workflow when a user clicks 'Change Password' on the Neon/ENW Account settings page .</t>
+  </si>
+  <si>
+    <t>1)       Sign-in with social and link existing steam account with matching email.
+2)       Sign-in with social account which already has linked steam account.</t>
+  </si>
+  <si>
+    <t>Sign-in with social with-out a linked steam account and link with non-matching email.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -330,6 +318,13 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -394,7 +389,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -413,6 +408,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -712,17 +710,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="70.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="70.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -742,7 +740,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="115.2">
+    <row r="2" spans="1:5" ht="135">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -759,7 +757,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="28.8">
+    <row r="3" spans="1:5" ht="30">
       <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
@@ -776,7 +774,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="43.2">
+    <row r="4" spans="1:5" ht="60">
       <c r="A4" s="2" t="s">
         <v>24</v>
       </c>
@@ -793,7 +791,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="28.8">
+    <row r="5" spans="1:5" ht="30">
       <c r="A5" s="2" t="s">
         <v>40</v>
       </c>
@@ -810,7 +808,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="28.8">
+    <row r="6" spans="1:5" ht="30">
       <c r="A6" s="2" t="s">
         <v>41</v>
       </c>
@@ -827,7 +825,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="43.2">
+    <row r="7" spans="1:5" ht="60">
       <c r="A7" s="2" t="s">
         <v>44</v>
       </c>
@@ -844,7 +842,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="57.6">
+    <row r="8" spans="1:5" ht="60">
       <c r="A8" s="2" t="s">
         <v>45</v>
       </c>
@@ -861,7 +859,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="28.8">
+    <row r="9" spans="1:5" ht="30">
       <c r="A9" s="2" t="s">
         <v>48</v>
       </c>
@@ -878,7 +876,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="129.6">
+    <row r="10" spans="1:5" ht="150">
       <c r="A10" s="2" t="s">
         <v>53</v>
       </c>
@@ -895,7 +893,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="100.8">
+    <row r="11" spans="1:5" ht="105">
       <c r="A11" s="2" t="s">
         <v>54</v>
       </c>
@@ -946,7 +944,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="201.6">
+    <row r="14" spans="1:5" ht="225">
       <c r="A14" s="2" t="s">
         <v>63</v>
       </c>
@@ -963,7 +961,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="144">
+    <row r="15" spans="1:5" ht="165">
       <c r="A15" s="2" t="s">
         <v>66</v>
       </c>
@@ -980,7 +978,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="43.2">
+    <row r="16" spans="1:5" ht="45">
       <c r="A16" s="2" t="s">
         <v>67</v>
       </c>
@@ -1014,7 +1012,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="28.8">
+    <row r="18" spans="1:5" ht="30">
       <c r="A18" s="2" t="s">
         <v>74</v>
       </c>
@@ -1031,7 +1029,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="216">
+    <row r="19" spans="1:5" ht="75">
       <c r="A19" s="2" t="s">
         <v>78</v>
       </c>
@@ -1039,58 +1037,58 @@
         <v>79</v>
       </c>
       <c r="C19" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="105">
+      <c r="A20" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D19" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="273.60000000000002">
-      <c r="A20" s="2" t="s">
+      <c r="B20" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="C20" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="30">
+      <c r="A21" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="B21" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="D20" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="28.8">
-      <c r="A21" s="2" t="s">
+      <c r="C21" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="D21" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="45">
+      <c r="A22" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="B22" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="D21" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="28.8">
-      <c r="A22" s="2" t="s">
+      <c r="C22" s="7" t="s">
         <v>87</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>89</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>3</v>
@@ -1113,13 +1111,13 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1253,12 +1251,12 @@
       <selection sqref="A1:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1398,7 +1396,7 @@
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
@@ -1469,12 +1467,12 @@
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1546,10 +1544,10 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">

</xml_diff>

<commit_message>
Modified test cases in ENWIAM module and in search module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENWIAM.xlsx
+++ b/src/test/resources/xls/ENWIAM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="96">
   <si>
     <t>TCID</t>
   </si>
@@ -298,6 +298,24 @@
   </si>
   <si>
     <t>Sign-in with social with-out a linked steam account and link with non-matching email.</t>
+  </si>
+  <si>
+    <t>ENWIAM100</t>
+  </si>
+  <si>
+    <t>ENWIAM101</t>
+  </si>
+  <si>
+    <t>OPQA-2119||OPQA-2287||OPQA-2293||OPQA-2305||OPQA-2308||OPQA-2319||OPQA-2336</t>
+  </si>
+  <si>
+    <t>Sign-in with social and link existing steam account with matching email.</t>
+  </si>
+  <si>
+    <t>OBT</t>
+  </si>
+  <si>
+    <t>OB T</t>
   </si>
 </sst>
 </file>
@@ -708,10 +726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1096,6 +1114,36 @@
       <c r="E22" s="2" t="s">
         <v>4</v>
       </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
test cases are to xml file
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENWIAM.xlsx
+++ b/src/test/resources/xls/ENWIAM.xlsx
@@ -309,13 +309,13 @@
     <t>OPQA-2119||OPQA-2287||OPQA-2293||OPQA-2305||OPQA-2308||OPQA-2319||OPQA-2336</t>
   </si>
   <si>
-    <t>Sign-in with social and link existing steam account with matching email.</t>
-  </si>
-  <si>
     <t>OBT</t>
   </si>
   <si>
-    <t>OB T</t>
+    <t xml:space="preserve">Verify that user is able to Sign-in with social and navigate to end note with-out a linked steam account and link with non-matching email for non market user.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that user is able to Sign-in with social and navigate to end note with-out a linked steam account and link with non-matching email for market user.  </t>
   </si>
 </sst>
 </file>
@@ -729,7 +729,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1115,27 +1115,27 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" ht="90">
       <c r="A23" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>93</v>
+      <c r="C23" s="7" t="s">
+        <v>94</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>3</v>
       </c>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" ht="45">
       <c r="A24" s="6" t="s">
         <v>91</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>95</v>

</xml_diff>

<commit_message>
New Testcase is added for Navigation
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENWIAM.xlsx
+++ b/src/test/resources/xls/ENWIAM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="99">
   <si>
     <t>TCID</t>
   </si>
@@ -316,6 +316,15 @@
   </si>
   <si>
     <t xml:space="preserve">Verify that user is able to Sign-in with social and navigate to end note with-out a linked steam account and link with non-matching email for market user.  </t>
+  </si>
+  <si>
+    <t>ENWIAM40</t>
+  </si>
+  <si>
+    <t>OPQA-2151</t>
+  </si>
+  <si>
+    <t>Verify that user is able to Navigate from Neon to EndNote</t>
   </si>
 </sst>
 </file>
@@ -726,10 +735,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1144,6 +1153,21 @@
         <v>3</v>
       </c>
       <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
New code for Neon Landing Page
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENWIAM.xlsx
+++ b/src/test/resources/xls/ENWIAM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="105">
   <si>
     <t>TCID</t>
   </si>
@@ -325,6 +325,24 @@
   </si>
   <si>
     <t>Verify that user is able to Navigate from Neon to EndNote</t>
+  </si>
+  <si>
+    <t>ENWIAM41</t>
+  </si>
+  <si>
+    <t>Verify that the User is able to see 'Did you know? ...' Modal is displayed when user navigates from neon to ENW if Neon user has email same as existing steam acount</t>
+  </si>
+  <si>
+    <t>OPQA-2172 || OPQA-1859</t>
+  </si>
+  <si>
+    <t>ENWIAM50</t>
+  </si>
+  <si>
+    <t>Verify that Neon Landing page, displays Neon branding and marketing copy and also integration with Endnote</t>
+  </si>
+  <si>
+    <t>OPQA-1707</t>
   </si>
 </sst>
 </file>
@@ -735,16 +753,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="70.7109375" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -1056,7 +1074,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="75">
+    <row r="19" spans="1:5" ht="60">
       <c r="A19" s="2" t="s">
         <v>78</v>
       </c>
@@ -1073,7 +1091,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="105">
+    <row r="20" spans="1:5" ht="90">
       <c r="A20" s="2" t="s">
         <v>80</v>
       </c>
@@ -1168,6 +1186,36 @@
         <v>3</v>
       </c>
       <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="1:5" ht="45">
+      <c r="A26" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="1:5" ht="30">
+      <c r="A27" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
New test cases for ENWIAM module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENWIAM.xlsx
+++ b/src/test/resources/xls/ENWIAM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="111">
   <si>
     <t>TCID</t>
   </si>
@@ -339,10 +339,29 @@
     <t>ENWIAM50</t>
   </si>
   <si>
-    <t>Verify that Neon Landing page, displays Neon branding and marketing copy and also integration with Endnote</t>
-  </si>
-  <si>
-    <t>OPQA-1707</t>
+    <t>OPQA-1707||OPQA-1734</t>
+  </si>
+  <si>
+    <t>ENWIAM51</t>
+  </si>
+  <si>
+    <t>OPQA-1673 || OPQA-1681 || OPQA-1691 || OPQA-1817 || OPQA-3648 || OPQA-3649</t>
+  </si>
+  <si>
+    <t>Verify that Neon Landing page, displays Neon branding , marketing copy , New icon and also integration with Endnote</t>
+  </si>
+  <si>
+    <t>Verify that on ENW landing page displays,EndNote branding and marketing copy and integration with Project Neon</t>
+  </si>
+  <si>
+    <t>ENWIAM42</t>
+  </si>
+  <si>
+    <t>OPQA-3689|| OPQA-2172</t>
+  </si>
+  <si>
+    <t>Verify that the User is able to see 'Did you know? ...' Modal is displayed when user navigates from neon to ENW if Neon user has email same as existing steam acount (used to login ENW).
+Verify that User should be taken back to Neon Home page, When User clicks on Close '[X] ' button on linking modals while Navigation from Neon via clicking link to EndNote</t>
   </si>
 </sst>
 </file>
@@ -753,10 +772,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1198,24 +1217,54 @@
         <v>100</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:5" ht="30">
+    <row r="27" spans="1:5" ht="90">
       <c r="A27" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="1:5" ht="30">
+      <c r="A28" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B28" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5" ht="60">
+      <c r="A29" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="C27" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E27" s="2"/>
+      <c r="B29" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E29" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Enw script implementation - sruthi
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENWIAM.xlsx
+++ b/src/test/resources/xls/ENWIAM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="114">
   <si>
     <t>TCID</t>
   </si>
@@ -330,12 +330,6 @@
     <t>ENWIAM41</t>
   </si>
   <si>
-    <t>Verify that the User is able to see 'Did you know? ...' Modal is displayed when user navigates from neon to ENW if Neon user has email same as existing steam acount</t>
-  </si>
-  <si>
-    <t>OPQA-2172 || OPQA-1859</t>
-  </si>
-  <si>
     <t>ENWIAM50</t>
   </si>
   <si>
@@ -362,6 +356,21 @@
   <si>
     <t>Verify that the User is able to see 'Did you know? ...' Modal is displayed when user navigates from neon to ENW if Neon user has email same as existing steam acount (used to login ENW).
 Verify that User should be taken back to Neon Home page, When User clicks on Close '[X] ' button on linking modals while Navigation from Neon via clicking link to EndNote</t>
+  </si>
+  <si>
+    <t>ENWIAM43</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> OPQA-1859</t>
+  </si>
+  <si>
+    <t>Verify that user who signed in to Neon through social shall be able to navigate to ENW after providing steam password in the Linking Modal</t>
+  </si>
+  <si>
+    <t>Verify that the User is able to see message  "Your account registration has not yet been confirmed. Please click on the verification link you were sent by email from &lt;no-reply-email-address&gt;, or have a link resent.</t>
+  </si>
+  <si>
+    <t>OPQA-1686</t>
   </si>
 </sst>
 </file>
@@ -772,10 +781,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1206,15 +1215,15 @@
       </c>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="1:5" ht="45">
+    <row r="26" spans="1:5" ht="30">
       <c r="A26" s="6" t="s">
         <v>99</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>3</v>
@@ -1223,48 +1232,63 @@
     </row>
     <row r="27" spans="1:5" ht="90">
       <c r="A27" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C27" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="D27" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="1:5" ht="45">
+      <c r="A28" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="C27" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E27" s="2"/>
-    </row>
-    <row r="28" spans="1:5" ht="30">
-      <c r="A28" s="6" t="s">
+      <c r="B28" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5" ht="30">
+      <c r="A29" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="1:5" ht="60">
+      <c r="A30" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B30" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="C28" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E28" s="2"/>
-    </row>
-    <row r="29" spans="1:5" ht="60">
-      <c r="A29" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="B29" s="7" t="s">
+      <c r="C30" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="C29" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E29" s="2"/>
+      <c r="D30" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E30" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ENW linking scenarios and evicted account scenario
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENWIAM.xlsx
+++ b/src/test/resources/xls/ENWIAM.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="3900"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="126">
   <si>
     <t>TCID</t>
   </si>
@@ -272,9 +272,6 @@
     <t>ENWIAM0002</t>
   </si>
   <si>
-    <t>OPQA-2373 || OPQA-2375 || OPQA-2377 || OPQA-2379 || OPQA-2381 || OPQA-2383 || OPQA-2385 || OPQA-2404 || OPQA-2405</t>
-  </si>
-  <si>
     <t>ENWIAM018</t>
   </si>
   <si>
@@ -371,13 +368,53 @@
   </si>
   <si>
     <t>OPQA-1686</t>
+  </si>
+  <si>
+    <t>OPQA-2373 || OPQA-2375 || OPQA-2377 || OPQA-2379 || OPQA-2381 || OPQA-2383 || OPQA-2385 || OPQA-2404 || OPQA-2405 || OPQa-2399 || OPQa-2382 || OPQa-2374</t>
+  </si>
+  <si>
+    <t>ENWIAM0003</t>
+  </si>
+  <si>
+    <t>OPQA-2389</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that,when STeAM account is trying to be linked by the user is in a "locked" status,then the link should not be made and the user should be informed that the STeAM account is locked.
+</t>
+  </si>
+  <si>
+    <t>ENWIAM0004</t>
+  </si>
+  <si>
+    <t>OPQA-3662</t>
+  </si>
+  <si>
+    <t>Verify that,user should receive a general error page when user tries to sign into Neon using an evicted account.</t>
+  </si>
+  <si>
+    <t>ENWIAM0005</t>
+  </si>
+  <si>
+    <t>OPQA-2399</t>
+  </si>
+  <si>
+    <t>Verify that,the user should not be able to exit the STeAM account linking process through clicking anywhere on the page.</t>
+  </si>
+  <si>
+    <t>ENWIAM0006</t>
+  </si>
+  <si>
+    <t>OPQA-2352 || OPQA-2353 || OPQA-2354 || OPQA-2335 || OPQA-2339 || OPQA-2337</t>
+  </si>
+  <si>
+    <t>Verify that [X] and "not now" button is working while linking two social accounts.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -420,7 +457,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -443,17 +480,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -462,15 +488,11 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -483,7 +505,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -493,6 +515,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -571,6 +598,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -605,6 +633,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -780,23 +809,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A28" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="70.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.42578125" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="70.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.28515625" style="2" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -813,482 +843,530 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="135">
+    <row r="2" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="30">
+      <c r="D2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="60">
+      <c r="D3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30">
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30">
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="60">
+    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="60">
+    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="30">
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="150">
+    <row r="10" spans="1:5" ht="150" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="105">
+      <c r="D10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="D11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="D12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="225">
+      <c r="D13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="285" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="165">
+      <c r="D14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="45">
+      <c r="D15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="30">
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="60">
+    <row r="19" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="C19" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="90">
+      <c r="C19" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="B21" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="D20" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="30">
-      <c r="A21" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="45">
-      <c r="A22" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="90">
-      <c r="A23" s="6" t="s">
+      <c r="B23" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B24" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C24" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="D23" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E23" s="2"/>
-    </row>
-    <row r="24" spans="1:5" ht="45">
-      <c r="A24" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C24" s="10" t="s">
+      <c r="D24" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="D24" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E24" s="2"/>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="6" t="s">
+      <c r="B25" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="C25" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="D25" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="D25" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E25" s="2"/>
-    </row>
-    <row r="26" spans="1:5" ht="30">
-      <c r="A26" s="6" t="s">
+      <c r="B26" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E26" s="2"/>
-    </row>
-    <row r="27" spans="1:5" ht="90">
-      <c r="A27" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E27" s="2"/>
-    </row>
-    <row r="28" spans="1:5" ht="45">
-      <c r="A28" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E28" s="2"/>
-    </row>
-    <row r="29" spans="1:5" ht="30">
-      <c r="A29" s="6" t="s">
+      <c r="B29" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="C29" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="B30" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C30" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="D29" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E29" s="2"/>
-    </row>
-    <row r="30" spans="1:5" ht="60">
-      <c r="A30" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E30" s="2"/>
+      <c r="D30" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1297,14 +1375,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
@@ -1313,7 +1391,7 @@
     <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1333,7 +1411,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>246</v>
       </c>
@@ -1351,7 +1429,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>247</v>
       </c>
@@ -1369,7 +1447,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>248</v>
       </c>
@@ -1389,7 +1467,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>111</v>
       </c>
@@ -1397,17 +1475,17 @@
       <c r="C5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="4" t="s">
         <v>3</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>111</v>
       </c>
@@ -1415,10 +1493,10 @@
         <v>18</v>
       </c>
       <c r="C6" s="3"/>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="4" t="s">
         <v>3</v>
       </c>
       <c r="F6" s="2" t="s">
@@ -1437,14 +1515,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
@@ -1452,7 +1530,7 @@
     <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -1472,7 +1550,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>28</v>
       </c>
@@ -1492,7 +1570,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
@@ -1512,7 +1590,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>32</v>
       </c>
@@ -1532,7 +1610,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>34</v>
       </c>
@@ -1545,14 +1623,14 @@
       <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="4" t="s">
         <v>3</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>35</v>
       </c>
@@ -1565,7 +1643,7 @@
       <c r="D6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="4" t="s">
         <v>3</v>
       </c>
       <c r="F6" s="2" t="s">
@@ -1582,16 +1660,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1605,7 +1683,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>49</v>
       </c>
@@ -1619,7 +1697,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>50</v>
       </c>
@@ -1633,7 +1711,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>51</v>
       </c>
@@ -1653,14 +1731,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
@@ -1668,7 +1746,7 @@
     <col min="4" max="4" width="4.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1682,7 +1760,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>49</v>
       </c>
@@ -1696,7 +1774,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>50</v>
       </c>
@@ -1710,7 +1788,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>51</v>
       </c>
@@ -1730,20 +1808,20 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1757,7 +1835,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>91</v>
       </c>
@@ -1771,7 +1849,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>92</v>
       </c>
@@ -1785,7 +1863,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>93</v>
       </c>

</xml_diff>

<commit_message>
Testcase Id are added to excel files
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENWIAM.xlsx
+++ b/src/test/resources/xls/ENWIAM.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="3900"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="125">
   <si>
     <t>TCID</t>
   </si>
@@ -303,9 +303,6 @@
     <t>ENWIAM101</t>
   </si>
   <si>
-    <t>OPQA-2119||OPQA-2287||OPQA-2293||OPQA-2305||OPQA-2308||OPQA-2319||OPQA-2336</t>
-  </si>
-  <si>
     <t>OBT</t>
   </si>
   <si>
@@ -413,8 +410,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -598,7 +595,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -633,7 +629,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -809,14 +804,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A28" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.42578125" style="2" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="24.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
@@ -826,7 +821,7 @@
     <col min="6" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -843,7 +838,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="135">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -860,7 +855,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="30">
       <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
@@ -877,7 +872,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="60">
       <c r="A4" s="2" t="s">
         <v>24</v>
       </c>
@@ -894,7 +889,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="30">
       <c r="A5" s="2" t="s">
         <v>40</v>
       </c>
@@ -911,7 +906,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="30">
       <c r="A6" s="2" t="s">
         <v>41</v>
       </c>
@@ -928,7 +923,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="60">
       <c r="A7" s="2" t="s">
         <v>44</v>
       </c>
@@ -945,7 +940,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="60">
       <c r="A8" s="2" t="s">
         <v>45</v>
       </c>
@@ -962,7 +957,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="30">
       <c r="A9" s="2" t="s">
         <v>48</v>
       </c>
@@ -979,7 +974,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="150">
       <c r="A10" s="2" t="s">
         <v>53</v>
       </c>
@@ -996,7 +991,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="105">
       <c r="A11" s="2" t="s">
         <v>54</v>
       </c>
@@ -1013,7 +1008,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="2" t="s">
         <v>57</v>
       </c>
@@ -1030,7 +1025,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="2" t="s">
         <v>58</v>
       </c>
@@ -1047,7 +1042,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="285" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="225">
       <c r="A14" s="2" t="s">
         <v>63</v>
       </c>
@@ -1064,7 +1059,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="165">
       <c r="A15" s="2" t="s">
         <v>66</v>
       </c>
@@ -1081,7 +1076,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="45">
       <c r="A16" s="2" t="s">
         <v>67</v>
       </c>
@@ -1098,7 +1093,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="2" t="s">
         <v>70</v>
       </c>
@@ -1115,7 +1110,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="30">
       <c r="A18" s="2" t="s">
         <v>74</v>
       </c>
@@ -1132,7 +1127,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="60">
       <c r="A19" s="2" t="s">
         <v>78</v>
       </c>
@@ -1149,12 +1144,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="105">
       <c r="A20" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>88</v>
@@ -1166,7 +1161,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="30">
       <c r="A21" s="2" t="s">
         <v>81</v>
       </c>
@@ -1183,7 +1178,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="45">
       <c r="A22" s="2" t="s">
         <v>84</v>
       </c>
@@ -1200,7 +1195,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="45">
       <c r="A23" s="4" t="s">
         <v>89</v>
       </c>
@@ -1208,161 +1203,161 @@
         <v>91</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="45">
       <c r="A24" s="4" t="s">
         <v>90</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C24" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D24" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+      <c r="B25" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="C25" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="D25" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="30">
+      <c r="A26" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="D25" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+      <c r="B26" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="90">
+      <c r="A27" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="45">
+      <c r="A28" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="30">
+      <c r="A29" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
+      <c r="B29" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="C29" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="60">
+      <c r="A30" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="B30" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C30" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="D29" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>104</v>
-      </c>
       <c r="D30" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="60">
       <c r="A31" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="C31" s="5" t="s">
         <v>115</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>116</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="30">
       <c r="A32" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="C32" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="D32" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="30">
+      <c r="A33" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
+      <c r="B33" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="C33" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="D33" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="60">
+      <c r="A34" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
+      <c r="B34" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="C34" s="5" t="s">
         <v>124</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>125</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>3</v>
@@ -1375,14 +1370,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
@@ -1391,7 +1386,7 @@
     <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1411,7 +1406,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="3">
         <v>246</v>
       </c>
@@ -1429,7 +1424,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="3">
         <v>247</v>
       </c>
@@ -1447,7 +1442,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="3">
         <v>248</v>
       </c>
@@ -1467,7 +1462,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="2">
         <v>111</v>
       </c>
@@ -1485,7 +1480,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="2">
         <v>111</v>
       </c>
@@ -1515,14 +1510,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
@@ -1530,7 +1525,7 @@
     <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -1550,7 +1545,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>28</v>
       </c>
@@ -1570,7 +1565,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
@@ -1590,7 +1585,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
         <v>32</v>
       </c>
@@ -1610,7 +1605,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="3" t="s">
         <v>34</v>
       </c>
@@ -1630,7 +1625,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="3" t="s">
         <v>35</v>
       </c>
@@ -1660,16 +1655,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1683,7 +1678,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="2">
         <v>49</v>
       </c>
@@ -1697,7 +1692,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="2">
         <v>50</v>
       </c>
@@ -1711,7 +1706,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="2">
         <v>51</v>
       </c>
@@ -1731,14 +1726,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
@@ -1746,7 +1741,7 @@
     <col min="4" max="4" width="4.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1760,7 +1755,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="2">
         <v>49</v>
       </c>
@@ -1774,7 +1769,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="2">
         <v>50</v>
       </c>
@@ -1788,7 +1783,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="2">
         <v>51</v>
       </c>
@@ -1808,20 +1803,20 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1835,7 +1830,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="2">
         <v>91</v>
       </c>
@@ -1849,7 +1844,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="2">
         <v>92</v>
       </c>
@@ -1863,7 +1858,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="2">
         <v>93</v>
       </c>

</xml_diff>

<commit_message>
modified Xls file for search and enwiam modules
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENWIAM.xlsx
+++ b/src/test/resources/xls/ENWIAM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="126">
   <si>
     <t>TCID</t>
   </si>
@@ -303,9 +303,6 @@
     <t>ENWIAM101</t>
   </si>
   <si>
-    <t>OBT</t>
-  </si>
-  <si>
     <t xml:space="preserve">Verify that user is able to Sign-in with social and navigate to end note with-out a linked steam account and link with non-matching email for non market user.  </t>
   </si>
   <si>
@@ -405,6 +402,12 @@
   </si>
   <si>
     <t>Verify that [X] and "not now" button is working while linking two social accounts.</t>
+  </si>
+  <si>
+    <t>OPQA-1861||OPQA-2173||OPQA-2174||OPQA-1898</t>
+  </si>
+  <si>
+    <t>OPQA-1861||OPQA-2173||OPQA-2174||OPQA-1898||OPQA-3643</t>
   </si>
 </sst>
 </file>
@@ -807,8 +810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1149,7 +1152,7 @@
         <v>80</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>88</v>
@@ -1195,15 +1198,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="45">
+    <row r="23" spans="1:5" ht="60">
       <c r="A23" s="4" t="s">
         <v>89</v>
       </c>
       <c r="B23" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>92</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>3</v>
@@ -1214,10 +1217,10 @@
         <v>90</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>91</v>
+        <v>124</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>3</v>
@@ -1225,13 +1228,13 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="C25" s="8" t="s">
         <v>95</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>96</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>3</v>
@@ -1239,13 +1242,13 @@
     </row>
     <row r="26" spans="1:5" ht="30">
       <c r="A26" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C26" s="8" t="s">
         <v>108</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>109</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>3</v>
@@ -1253,13 +1256,13 @@
     </row>
     <row r="27" spans="1:5" ht="90">
       <c r="A27" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="C27" s="8" t="s">
         <v>105</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>106</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>3</v>
@@ -1267,13 +1270,13 @@
     </row>
     <row r="28" spans="1:5" ht="45">
       <c r="A28" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>3</v>
@@ -1281,13 +1284,13 @@
     </row>
     <row r="29" spans="1:5" ht="30">
       <c r="A29" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>99</v>
-      </c>
       <c r="C29" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>3</v>
@@ -1295,13 +1298,13 @@
     </row>
     <row r="30" spans="1:5" ht="60">
       <c r="A30" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>101</v>
-      </c>
       <c r="C30" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>3</v>
@@ -1309,13 +1312,13 @@
     </row>
     <row r="31" spans="1:5" ht="60">
       <c r="A31" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="C31" s="5" t="s">
         <v>114</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>115</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>28</v>
@@ -1323,13 +1326,13 @@
     </row>
     <row r="32" spans="1:5" ht="30">
       <c r="A32" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="C32" s="5" t="s">
         <v>117</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>118</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>3</v>
@@ -1337,13 +1340,13 @@
     </row>
     <row r="33" spans="1:4" ht="30">
       <c r="A33" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="C33" s="5" t="s">
         <v>120</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>121</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>3</v>
@@ -1351,13 +1354,13 @@
     </row>
     <row r="34" spans="1:4" ht="60">
       <c r="A34" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="C34" s="5" t="s">
         <v>123</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>124</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
New Scripts for Forward Merge Scenarios and ContactCustomerSupport Merge Scenarios.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENWIAM.xlsx
+++ b/src/test/resources/xls/ENWIAM.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="3900"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="135">
   <si>
     <t>TCID</t>
   </si>
@@ -409,12 +409,39 @@
   <si>
     <t>OPQA-1861||OPQA-2173||OPQA-2174||OPQA-1898||OPQA-3643</t>
   </si>
+  <si>
+    <t>ENWIAM52</t>
+  </si>
+  <si>
+    <t>OPQA-2033</t>
+  </si>
+  <si>
+    <t>From Neon, Verify that user is informed to contact Customer support through an inline error message, when Neon Active STeAM account and  Neon Active Facebook account are attempted to merge.</t>
+  </si>
+  <si>
+    <t>ENWIAM53</t>
+  </si>
+  <si>
+    <t>OPQA-1980</t>
+  </si>
+  <si>
+    <t>From Neon,Verify that the system is able to merge New STeAM account and Activated Facebook account and after merge verify STeAM TRUID is changed</t>
+  </si>
+  <si>
+    <t>ENWIAM54</t>
+  </si>
+  <si>
+    <t>OPQA-1999</t>
+  </si>
+  <si>
+    <t>From Neon, Verify that the system is able to merge Neon Active STeAM account and New Facebook account</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -598,6 +625,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -632,6 +660,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -807,14 +836,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" style="2" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="24.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
@@ -824,7 +853,7 @@
     <col min="6" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -841,7 +870,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="135">
+    <row r="2" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -858,7 +887,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
@@ -875,7 +904,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="60">
+    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>24</v>
       </c>
@@ -892,7 +921,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30">
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>40</v>
       </c>
@@ -909,7 +938,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30">
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>41</v>
       </c>
@@ -926,7 +955,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="60">
+    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>44</v>
       </c>
@@ -943,7 +972,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="60">
+    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>45</v>
       </c>
@@ -960,7 +989,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="30">
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>48</v>
       </c>
@@ -977,7 +1006,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="150">
+    <row r="10" spans="1:5" ht="150" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>53</v>
       </c>
@@ -994,7 +1023,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="105">
+    <row r="11" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>54</v>
       </c>
@@ -1011,7 +1040,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>57</v>
       </c>
@@ -1028,7 +1057,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>58</v>
       </c>
@@ -1045,7 +1074,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="225">
+    <row r="14" spans="1:5" ht="285" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>63</v>
       </c>
@@ -1062,7 +1091,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="165">
+    <row r="15" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>66</v>
       </c>
@@ -1079,7 +1108,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="45">
+    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>67</v>
       </c>
@@ -1096,7 +1125,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>70</v>
       </c>
@@ -1113,7 +1142,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="30">
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>74</v>
       </c>
@@ -1130,7 +1159,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="60">
+    <row r="19" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>78</v>
       </c>
@@ -1147,7 +1176,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="105">
+    <row r="20" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>80</v>
       </c>
@@ -1164,7 +1193,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="30">
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>81</v>
       </c>
@@ -1181,7 +1210,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="45">
+    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>84</v>
       </c>
@@ -1198,7 +1227,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="60">
+    <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>89</v>
       </c>
@@ -1212,7 +1241,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="45">
+    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>90</v>
       </c>
@@ -1226,7 +1255,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>93</v>
       </c>
@@ -1240,7 +1269,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="30">
+    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>96</v>
       </c>
@@ -1254,7 +1283,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="90">
+    <row r="27" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>103</v>
       </c>
@@ -1268,7 +1297,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="45">
+    <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>106</v>
       </c>
@@ -1282,7 +1311,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="30">
+    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>97</v>
       </c>
@@ -1296,7 +1325,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="60">
+    <row r="30" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>99</v>
       </c>
@@ -1310,59 +1339,101 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="60">
-      <c r="A31" s="4" t="s">
+    <row r="31" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B34" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C34" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D34" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="30">
-      <c r="A32" s="4" t="s">
+    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B35" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C35" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="30">
-      <c r="A33" s="4" t="s">
+      <c r="D35" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B36" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C36" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="60">
-      <c r="A34" s="4" t="s">
+      <c r="D36" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B37" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C37" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D37" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1373,14 +1444,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
@@ -1389,7 +1460,7 @@
     <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1409,7 +1480,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>246</v>
       </c>
@@ -1427,7 +1498,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>247</v>
       </c>
@@ -1445,7 +1516,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>248</v>
       </c>
@@ -1465,7 +1536,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>111</v>
       </c>
@@ -1483,7 +1554,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>111</v>
       </c>
@@ -1513,14 +1584,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
@@ -1528,7 +1599,7 @@
     <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -1548,7 +1619,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>28</v>
       </c>
@@ -1568,7 +1639,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
@@ -1588,7 +1659,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>32</v>
       </c>
@@ -1608,7 +1679,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>34</v>
       </c>
@@ -1628,7 +1699,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>35</v>
       </c>
@@ -1658,16 +1729,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1681,7 +1752,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>49</v>
       </c>
@@ -1695,7 +1766,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>50</v>
       </c>
@@ -1709,7 +1780,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>51</v>
       </c>
@@ -1729,14 +1800,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
@@ -1744,7 +1815,7 @@
     <col min="4" max="4" width="4.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1758,7 +1829,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>49</v>
       </c>
@@ -1772,7 +1843,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>50</v>
       </c>
@@ -1786,7 +1857,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>51</v>
       </c>
@@ -1806,20 +1877,20 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1833,7 +1904,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>91</v>
       </c>
@@ -1847,7 +1918,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>92</v>
       </c>
@@ -1861,7 +1932,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>93</v>
       </c>

</xml_diff>

<commit_message>
Added Jira ID for RandomMerge Testcase
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENWIAM.xlsx
+++ b/src/test/resources/xls/ENWIAM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="138">
   <si>
     <t>TCID</t>
   </si>
@@ -435,6 +435,15 @@
   </si>
   <si>
     <t>From Neon, Verify that the system is able to merge Neon Active STeAM account and New Facebook account</t>
+  </si>
+  <si>
+    <t>ENWIAM55</t>
+  </si>
+  <si>
+    <t>OPQA-2036</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> From Neon, Verify that system is able to merge Activated STeAM account and Activated Facebook account and after merge verify STeAM TRUID is changed</t>
   </si>
 </sst>
 </file>
@@ -837,10 +846,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1381,59 +1390,73 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
+    <row r="34" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B35" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C35" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D35" s="2" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C37" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
+      <c r="D37" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B38" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C38" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D38" s="2" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed ENW Linking scripts in ENWIAM Module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENWIAM.xlsx
+++ b/src/test/resources/xls/ENWIAM.xlsx
@@ -848,8 +848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1415,7 +1415,7 @@
         <v>114</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
linking with unverified steam
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENWIAM.xlsx
+++ b/src/test/resources/xls/ENWIAM.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="3900"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="147">
   <si>
     <t>TCID</t>
   </si>
@@ -290,13 +290,6 @@
     <t>The system should send the user through the Neon/ENW password reset workflow when a user clicks 'Change Password' on the Neon/ENW Account settings page .</t>
   </si>
   <si>
-    <t>1)       Sign-in with social and link existing steam account with matching email.
-2)       Sign-in with social account which already has linked steam account.</t>
-  </si>
-  <si>
-    <t>Sign-in with social with-out a linked steam account and link with non-matching email.</t>
-  </si>
-  <si>
     <t>ENWIAM100</t>
   </si>
   <si>
@@ -364,9 +357,6 @@
     <t>OPQA-1686</t>
   </si>
   <si>
-    <t>OPQA-2373 || OPQA-2375 || OPQA-2377 || OPQA-2379 || OPQA-2381 || OPQA-2383 || OPQA-2385 || OPQA-2404 || OPQA-2405 || OPQa-2399 || OPQa-2382 || OPQa-2374</t>
-  </si>
-  <si>
     <t>ENWIAM0003</t>
   </si>
   <si>
@@ -444,6 +434,44 @@
   </si>
   <si>
     <t xml:space="preserve"> From Neon, Verify that system is able to merge Activated STeAM account and Activated Facebook account and after merge verify STeAM TRUID is changed</t>
+  </si>
+  <si>
+    <t>ENWIAM0007</t>
+  </si>
+  <si>
+    <t>ENWIAM0008</t>
+  </si>
+  <si>
+    <t>ENWIAM0009</t>
+  </si>
+  <si>
+    <t>Verify unverified account is not able to linked</t>
+  </si>
+  <si>
+    <t>OPQA-1862 || OPQA-1863 || OPQA-1864  || OPQA-1869</t>
+  </si>
+  <si>
+    <t>1)       Sign-in with Linkedin and link existing steam account with matching email.
+2)       Sign-in with LinkedIn account which already has linked steam account.</t>
+  </si>
+  <si>
+    <t>1)       Sign-in with Facebook and link existing steam account with matching email.
+2)       Sign-in with Facebook account which already has linked steam account.</t>
+  </si>
+  <si>
+    <t>Sign-in with LinkedIn with-out a linked steam account and link with non-matching email.</t>
+  </si>
+  <si>
+    <t>Sign-in with Facebook with-out a linked steam account and link with non-matching email.</t>
+  </si>
+  <si>
+    <t>OPQA-2381 || OPQA-2383 || OPQA-2385 || OPQA-2404 || OPQA-2405 || OPQa-2399 || OPQa-2382 || OPQa-2374</t>
+  </si>
+  <si>
+    <t>OPQA-2373 || OPQA-2375 || OPQA-2377 || OPQA-2379 || OPQA-2404 || OPQA-2405 || OPQa-2399 || OPQa-2382 || OPQa-2374</t>
+  </si>
+  <si>
+    <t>OPQA-1848</t>
   </si>
 </sst>
 </file>
@@ -555,6 +583,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -602,7 +633,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -637,7 +668,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -846,10 +877,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1176,7 +1207,7 @@
         <v>79</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>87</v>
+        <v>141</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>3</v>
@@ -1185,15 +1216,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>111</v>
+        <v>145</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>88</v>
+        <v>143</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>3</v>
@@ -1238,13 +1269,13 @@
     </row>
     <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>89</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>91</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>3</v>
@@ -1252,13 +1283,13 @@
     </row>
     <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C24" s="8" t="s">
         <v>90</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>92</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>3</v>
@@ -1266,13 +1297,13 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C25" s="8" t="s">
         <v>93</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>95</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>3</v>
@@ -1280,13 +1311,13 @@
     </row>
     <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>3</v>
@@ -1294,13 +1325,13 @@
     </row>
     <row r="27" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C27" s="8" t="s">
         <v>103</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>105</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>3</v>
@@ -1308,13 +1339,13 @@
     </row>
     <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>3</v>
@@ -1322,13 +1353,13 @@
     </row>
     <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>3</v>
@@ -1336,13 +1367,13 @@
     </row>
     <row r="30" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B30" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C30" s="8" t="s">
         <v>100</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>102</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>3</v>
@@ -1350,13 +1381,13 @@
     </row>
     <row r="31" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D31" s="8" t="s">
         <v>3</v>
@@ -1364,13 +1395,13 @@
     </row>
     <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D32" s="8" t="s">
         <v>3</v>
@@ -1378,13 +1409,13 @@
     </row>
     <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D33" s="8" t="s">
         <v>3</v>
@@ -1392,13 +1423,13 @@
     </row>
     <row r="34" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D34" s="8" t="s">
         <v>3</v>
@@ -1406,13 +1437,13 @@
     </row>
     <row r="35" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>3</v>
@@ -1420,13 +1451,13 @@
     </row>
     <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>3</v>
@@ -1434,13 +1465,13 @@
     </row>
     <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>3</v>
@@ -1448,15 +1479,57 @@
     </row>
     <row r="38" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D38" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New Script for Random merge - ENW
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENWIAM.xlsx
+++ b/src/test/resources/xls/ENWIAM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="162">
   <si>
     <t>TCID</t>
   </si>
@@ -508,6 +508,15 @@
   </si>
   <si>
     <t xml:space="preserve"> ENW side Forward Merge: Facebook-New Steam-Activated </t>
+  </si>
+  <si>
+    <t>ENWIAM59</t>
+  </si>
+  <si>
+    <t>OPQA-2924</t>
+  </si>
+  <si>
+    <t>From ENW,verify that system is able to merge Activated STeAM account and Activated Facebook account and after merge verify STeAM TRUID is changed</t>
   </si>
 </sst>
 </file>
@@ -913,10 +922,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1513,29 +1522,29 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
+    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B39" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C39" s="5" t="s">
         <v>111</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>114</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>3</v>
@@ -1543,85 +1552,99 @@
     </row>
     <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B41" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="C41" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="D40" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
+      <c r="D41" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B42" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C42" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="D41" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
+      <c r="D42" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="B42" s="8" t="s">
+      <c r="B43" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="C42" s="8" t="s">
+      <c r="C43" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="D42" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
+      <c r="D43" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="B43" s="8" t="s">
+      <c r="B44" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="C43" s="10" t="s">
+      <c r="C44" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="D43" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
+      <c r="D44" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B45" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="C45" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="D44" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
+      <c r="D45" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B46" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C46" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D46" s="2" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added ne scripts for ENWIAM
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENWIAM.xlsx
+++ b/src/test/resources/xls/ENWIAM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="171">
   <si>
     <t>TCID</t>
   </si>
@@ -527,12 +527,30 @@
   <si>
     <t>ENW automated Merge</t>
   </si>
+  <si>
+    <t>ENWIAM00015</t>
+  </si>
+  <si>
+    <t>OPQA-1870||OPQA-1874</t>
+  </si>
+  <si>
+    <t>Verify that If the STeAM account that is trying to be linked/merged by the user is in a "locked"/Suspended status, then the link/merge shall not be made and the user shall be informed that the STeAM account is locked.</t>
+  </si>
+  <si>
+    <t>ENWIAM00016</t>
+  </si>
+  <si>
+    <t>OPQA-2362||OPQA-2359</t>
+  </si>
+  <si>
+    <t>Verify that upon a successful sign-in for the first time on the ENW landing screen using STeAM, the user shall be prompted to link existing Neon accounts that have the same email address as the newly registered account</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -550,6 +568,13 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -606,7 +631,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -624,6 +649,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -959,10 +987,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+      <selection activeCell="A48" sqref="A48:XFD48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1700,6 +1728,34 @@
       </c>
       <c r="E47" s="8"/>
       <c r="F47" s="8"/>
+    </row>
+    <row r="48" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C48" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added opqa-3331 to enwiam51
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENWIAM.xlsx
+++ b/src/test/resources/xls/ENWIAM.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="3900"/>
@@ -14,7 +14,7 @@
     <sheet name="ENWIAM005" sheetId="9" r:id="rId5"/>
     <sheet name="ENWIAM016" sheetId="10" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -323,13 +323,7 @@
     <t>ENWIAM51</t>
   </si>
   <si>
-    <t>OPQA-1673 || OPQA-1681 || OPQA-1691 || OPQA-1817 || OPQA-3648 || OPQA-3649</t>
-  </si>
-  <si>
     <t>Verify that Neon Landing page, displays Neon branding , marketing copy , New icon and also integration with Endnote</t>
-  </si>
-  <si>
-    <t>Verify that on ENW landing page displays,EndNote branding and marketing copy and integration with Project Neon</t>
   </si>
   <si>
     <t>ENWIAM42</t>
@@ -445,9 +439,6 @@
     <t>ENWIAM0009</t>
   </si>
   <si>
-    <t>Verify unverified account is not able to linked</t>
-  </si>
-  <si>
     <t>OPQA-1862 || OPQA-1863 || OPQA-1864  || OPQA-1869</t>
   </si>
   <si>
@@ -471,9 +462,6 @@
     <t>OPQA-2373 || OPQA-2375 || OPQA-2377 || OPQA-2379 || OPQA-2404 || OPQA-2405 || OPQa-2399 || OPQa-2382 || OPQa-2374</t>
   </si>
   <si>
-    <t>OPQA-1848</t>
-  </si>
-  <si>
     <t>ENWIAM56</t>
   </si>
   <si>
@@ -553,6 +541,19 @@
   </si>
   <si>
     <t>Verify that If the STeAM account that is trying to be linked/merged by the user is in a "locked" status, then the link/merge shall not be made and the user shall be informed that the STeAM account is locked.</t>
+  </si>
+  <si>
+    <t>Verify that,an error message should display as "email activation",when
+User did'nt activate the link in that respective mail after completing the registration process in ENW.||Verify that,when STeAM account' email is trying to be linked by the user is in an "unverified" status, then the link should not be made and the user should be provided the ability to resend activation email and navigate back to ENW landing page.</t>
+  </si>
+  <si>
+    <t>OPQA-1848||OPQA-2391</t>
+  </si>
+  <si>
+    <t>OPQA-1673 || OPQA-1681 || OPQA-1691 || OPQA-1817 || OPQA-3648 || OPQA-3649||OPQA-3331</t>
+  </si>
+  <si>
+    <t>Verify that on ENW landing page displays,EndNote branding and marketing copy and integration with Project Neon||Verify that user is able to see login through Shibboleth link in ENW Login screen and upon clicking the link it should navigate to proper URL to Login</t>
   </si>
 </sst>
 </file>
@@ -752,7 +753,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -787,7 +788,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -998,8 +999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50:XFD50"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1326,7 +1327,7 @@
         <v>79</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>3</v>
@@ -1340,10 +1341,10 @@
         <v>80</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>3</v>
@@ -1391,7 +1392,7 @@
         <v>87</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>89</v>
@@ -1405,7 +1406,7 @@
         <v>88</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>90</v>
@@ -1433,10 +1434,10 @@
         <v>94</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>3</v>
@@ -1444,13 +1445,13 @@
     </row>
     <row r="27" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C27" s="8" t="s">
         <v>101</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>103</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>3</v>
@@ -1458,13 +1459,13 @@
     </row>
     <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>3</v>
@@ -1478,7 +1479,7 @@
         <v>96</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>3</v>
@@ -1489,10 +1490,10 @@
         <v>97</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>98</v>
+        <v>172</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>100</v>
+        <v>173</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>3</v>
@@ -1500,13 +1501,13 @@
     </row>
     <row r="31" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C31" s="8" t="s">
         <v>123</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>125</v>
       </c>
       <c r="D31" s="8" t="s">
         <v>3</v>
@@ -1514,13 +1515,13 @@
     </row>
     <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C32" s="8" t="s">
         <v>126</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>128</v>
       </c>
       <c r="D32" s="8" t="s">
         <v>3</v>
@@ -1528,13 +1529,13 @@
     </row>
     <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C33" s="8" t="s">
         <v>129</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>131</v>
       </c>
       <c r="D33" s="8" t="s">
         <v>3</v>
@@ -1542,13 +1543,13 @@
     </row>
     <row r="34" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C34" s="8" t="s">
         <v>132</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>134</v>
       </c>
       <c r="D34" s="8" t="s">
         <v>3</v>
@@ -1556,13 +1557,13 @@
     </row>
     <row r="35" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D35" s="8" t="s">
         <v>3</v>
@@ -1570,13 +1571,13 @@
     </row>
     <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D36" s="8" t="s">
         <v>3</v>
@@ -1584,13 +1585,13 @@
     </row>
     <row r="37" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D37" s="8" t="s">
         <v>3</v>
@@ -1598,13 +1599,13 @@
     </row>
     <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D38" s="8" t="s">
         <v>3</v>
@@ -1612,13 +1613,13 @@
     </row>
     <row r="39" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C39" s="5" t="s">
         <v>109</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>111</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>3</v>
@@ -1626,13 +1627,13 @@
     </row>
     <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>112</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>114</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>3</v>
@@ -1640,13 +1641,13 @@
     </row>
     <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C41" s="5" t="s">
         <v>115</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>117</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>3</v>
@@ -1654,13 +1655,13 @@
     </row>
     <row r="42" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C42" s="5" t="s">
         <v>118</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>120</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>3</v>
@@ -1668,13 +1669,13 @@
     </row>
     <row r="43" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>3</v>
@@ -1682,27 +1683,27 @@
     </row>
     <row r="44" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>146</v>
+        <v>171</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>138</v>
+        <v>170</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>3</v>
@@ -1710,13 +1711,13 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>3</v>
@@ -1724,13 +1725,13 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>3</v>
@@ -1740,13 +1741,13 @@
     </row>
     <row r="48" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B48" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C48" s="11" t="s">
         <v>166</v>
-      </c>
-      <c r="C48" s="11" t="s">
-        <v>170</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>3</v>
@@ -1754,13 +1755,13 @@
     </row>
     <row r="49" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>3</v>
@@ -1768,13 +1769,13 @@
     </row>
     <row r="50" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
added jiraids to enwiam.xls
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENWIAM.xlsx
+++ b/src/test/resources/xls/ENWIAM.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="3900"/>
@@ -57,21 +57,6 @@
     <t>ENWIAM001</t>
   </si>
   <si>
-    <t>OPQA-1719||
-OPQA-1676||OPQA-1744||
-OPQA-1760||OPQA-1763
-||OPQA-1766</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verify that ENW registration screen should be displayed and User should be able to enter email address (required), name (required), and password (required).||Verify that "Sign up" link should be displayed on ENW registration page .||Verify that the user should be able click on "sign up" button after filling the above fields correctly.||Verify that user should get an Email verification Link on the registered Email Id .||Verify that after clicking verification link user should get the message as" Success!You have successfully activated your account. Please sign in."||Verify that after completion of verification process,user should be able to sign into ENW </t>
-  </si>
-  <si>
-    <t>OPQA-1731</t>
-  </si>
-  <si>
-    <t>Verify that email address field should be in standard email ID format .Email address fields should be mandatory.</t>
-  </si>
-  <si>
     <t>SUFFIX</t>
   </si>
   <si>
@@ -555,6 +540,21 @@
   <si>
     <t>Verify that [X] and "not now" button is working while linking two social accounts.
 || Verify that,the user should not be able to exit the STeAM account linking process through clicking anywhere on the page.</t>
+  </si>
+  <si>
+    <t>OPQA-1731||OPQA-2406</t>
+  </si>
+  <si>
+    <t>Verify that email address field should be in standard email ID format .Email address fields should be mandatory.||Verify that,the system should add the non-matching email as an alternate email under the Neon account,after providing correct credentials of an existing STeAM account with a non-matching email address</t>
+  </si>
+  <si>
+    <t>Verify that ENW registration screen should be displayed and User should be able to enter email address (required), name (required), and password (required).||Verify that "Sign up" link should be displayed on ENW registration page .||Verify that the user should be able click on "sign up" button after filling the above fields correctly.||Verify that user should get an Email verification Link on the registered Email Id .||Verify that after clicking verification link user should get the message as" Success!You have successfully activated your account. Please sign in."||Verify that after completion of verification process,user should be able to sign into ENW ||Verify that after successful registration on the ENW landing screen using Facebook, users who already has Steam account with the same email address are prompted to link their Steam account with the newly created Facebook account.</t>
+  </si>
+  <si>
+    <t>OPQA-1719||
+OPQA-1676||OPQA-1744||
+OPQA-1760||OPQA-1763
+||OPQA-1766||OPQA-2038</t>
   </si>
 </sst>
 </file>
@@ -754,7 +754,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -789,7 +789,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1000,8 +1000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1031,15 +1031,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="195" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>12</v>
+        <v>173</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>13</v>
+        <v>172</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>3</v>
@@ -1048,15 +1048,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>14</v>
+        <v>170</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>15</v>
+        <v>171</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>3</v>
@@ -1067,13 +1067,13 @@
     </row>
     <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>3</v>
@@ -1084,13 +1084,13 @@
     </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>3</v>
@@ -1101,13 +1101,13 @@
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>3</v>
@@ -1118,13 +1118,13 @@
     </row>
     <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>3</v>
@@ -1135,13 +1135,13 @@
     </row>
     <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>3</v>
@@ -1152,13 +1152,13 @@
     </row>
     <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>3</v>
@@ -1169,13 +1169,13 @@
     </row>
     <row r="10" spans="1:5" ht="150" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>3</v>
@@ -1186,13 +1186,13 @@
     </row>
     <row r="11" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>3</v>
@@ -1203,13 +1203,13 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>3</v>
@@ -1220,13 +1220,13 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="8" t="s">
         <v>58</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>62</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>3</v>
@@ -1237,13 +1237,13 @@
     </row>
     <row r="14" spans="1:5" ht="285" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>3</v>
@@ -1254,13 +1254,13 @@
     </row>
     <row r="15" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" s="8" t="s">
         <v>73</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>77</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>3</v>
@@ -1271,13 +1271,13 @@
     </row>
     <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>3</v>
@@ -1288,13 +1288,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>3</v>
@@ -1305,13 +1305,13 @@
     </row>
     <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>3</v>
@@ -1322,13 +1322,13 @@
     </row>
     <row r="19" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>3</v>
@@ -1339,13 +1339,13 @@
     </row>
     <row r="20" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>3</v>
@@ -1356,13 +1356,13 @@
     </row>
     <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>3</v>
@@ -1373,13 +1373,13 @@
     </row>
     <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>3</v>
@@ -1390,13 +1390,13 @@
     </row>
     <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>3</v>
@@ -1404,13 +1404,13 @@
     </row>
     <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>3</v>
@@ -1418,13 +1418,13 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>3</v>
@@ -1432,13 +1432,13 @@
     </row>
     <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>3</v>
@@ -1446,13 +1446,13 @@
     </row>
     <row r="27" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>3</v>
@@ -1460,13 +1460,13 @@
     </row>
     <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>106</v>
-      </c>
       <c r="C28" s="8" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>3</v>
@@ -1474,13 +1474,13 @@
     </row>
     <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>3</v>
@@ -1488,13 +1488,13 @@
     </row>
     <row r="30" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>3</v>
@@ -1502,13 +1502,13 @@
     </row>
     <row r="31" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D31" s="8" t="s">
         <v>3</v>
@@ -1516,13 +1516,13 @@
     </row>
     <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D32" s="8" t="s">
         <v>3</v>
@@ -1530,13 +1530,13 @@
     </row>
     <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D33" s="8" t="s">
         <v>3</v>
@@ -1544,13 +1544,13 @@
     </row>
     <row r="34" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D34" s="8" t="s">
         <v>3</v>
@@ -1558,13 +1558,13 @@
     </row>
     <row r="35" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D35" s="8" t="s">
         <v>3</v>
@@ -1572,13 +1572,13 @@
     </row>
     <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D36" s="8" t="s">
         <v>3</v>
@@ -1586,13 +1586,13 @@
     </row>
     <row r="37" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D37" s="8" t="s">
         <v>3</v>
@@ -1600,13 +1600,13 @@
     </row>
     <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D38" s="8" t="s">
         <v>3</v>
@@ -1614,13 +1614,13 @@
     </row>
     <row r="39" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>3</v>
@@ -1628,13 +1628,13 @@
     </row>
     <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>3</v>
@@ -1642,13 +1642,13 @@
     </row>
     <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>3</v>
@@ -1656,13 +1656,13 @@
     </row>
     <row r="42" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>3</v>
@@ -1670,13 +1670,13 @@
     </row>
     <row r="43" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="C43" s="8" t="s">
         <v>132</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>136</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>3</v>
@@ -1684,13 +1684,13 @@
     </row>
     <row r="44" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>3</v>
@@ -1698,13 +1698,13 @@
     </row>
     <row r="45" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>3</v>
@@ -1712,13 +1712,13 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>3</v>
@@ -1726,13 +1726,13 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>3</v>
@@ -1742,13 +1742,13 @@
     </row>
     <row r="48" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B48" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C48" s="11" t="s">
         <v>161</v>
-      </c>
-      <c r="C48" s="11" t="s">
-        <v>165</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>3</v>
@@ -1756,13 +1756,13 @@
     </row>
     <row r="49" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>3</v>
@@ -1770,13 +1770,13 @@
     </row>
     <row r="50" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>3</v>
@@ -1810,10 +1810,10 @@
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>5</v>
@@ -1830,7 +1830,7 @@
         <v>246</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3" t="s">
@@ -1848,7 +1848,7 @@
         <v>247</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
@@ -1866,10 +1866,10 @@
         <v>248</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>7</v>
@@ -1887,7 +1887,7 @@
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>7</v>
@@ -1904,7 +1904,7 @@
         <v>111</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="7" t="s">
@@ -1946,13 +1946,13 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>5</v>
@@ -1966,10 +1966,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -1981,15 +1981,15 @@
         <v>3</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C3" s="2">
         <v>2</v>
@@ -2006,10 +2006,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C4" s="2">
         <v>3</v>
@@ -2026,10 +2026,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C5" s="2">
         <v>4</v>
@@ -2046,10 +2046,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C6" s="2">
         <v>5</v>

</xml_diff>

<commit_message>
added jiraids to enwiam
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENWIAM.xlsx
+++ b/src/test/resources/xls/ENWIAM.xlsx
@@ -14,7 +14,7 @@
     <sheet name="ENWIAM005" sheetId="9" r:id="rId5"/>
     <sheet name="ENWIAM016" sheetId="10" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -175,13 +175,7 @@
     <t>ENWIAM012</t>
   </si>
   <si>
-    <t>OPQA-2015</t>
-  </si>
-  <si>
     <t>Verify that User is able to sign-into EndNote Web using Facebook</t>
-  </si>
-  <si>
-    <t>OPQA-2016</t>
   </si>
   <si>
     <t>Verify that User is able to sign-into EndNote Web using Linkedn</t>
@@ -423,9 +417,6 @@
     <t>OPQA-2381 || OPQA-2383 || OPQA-2385 || OPQA-2404 || OPQA-2405 || OPQa-2399 || OPQa-2382 || OPQa-2374</t>
   </si>
   <si>
-    <t>OPQA-2373 || OPQA-2375 || OPQA-2377 || OPQA-2379 || OPQA-2404 || OPQA-2405 || OPQa-2399 || OPQa-2382 || OPQa-2374</t>
-  </si>
-  <si>
     <t>ENWIAM56</t>
   </si>
   <si>
@@ -483,9 +474,6 @@
     <t>ENWIAM00015</t>
   </si>
   <si>
-    <t>OPQA-1870||OPQA-1874</t>
-  </si>
-  <si>
     <t>ENWIAM00016</t>
   </si>
   <si>
@@ -499,9 +487,6 @@
   </si>
   <si>
     <t>ENWIAM00017</t>
-  </si>
-  <si>
-    <t>OPQA-1870</t>
   </si>
   <si>
     <t>Verify that If the STeAM account that is trying to be linked/merged by the user is in a "locked" status, then the link/merge shall not be made and the user shall be informed that the STeAM account is locked.</t>
@@ -555,6 +540,21 @@
   </si>
   <si>
     <t>OPQA-1731||OPQA-2406||OPQA-2382||OPQA-2170</t>
+  </si>
+  <si>
+    <t>OPQA-2015||OPQA-3650</t>
+  </si>
+  <si>
+    <t>OPQA-2016||OPQA-3650</t>
+  </si>
+  <si>
+    <t>OPQA-1870||OPQA-3580</t>
+  </si>
+  <si>
+    <t>OPQA-2373 || OPQA-2375 || OPQA-2377 || OPQA-2379 || OPQA-2404 || OPQA-2405 || OPQa-2399 || OPQA-2382 || OPQA-2374</t>
+  </si>
+  <si>
+    <t>OPQA-1870||OPQA-1874||OPQA-2390||OPQA-1768||OPQA-1777</t>
   </si>
 </sst>
 </file>
@@ -1000,8 +1000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1036,10 +1036,10 @@
         <v>11</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>3</v>
@@ -1053,10 +1053,10 @@
         <v>17</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>3</v>
@@ -1070,10 +1070,10 @@
         <v>18</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>3</v>
@@ -1189,10 +1189,10 @@
         <v>48</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>3</v>
@@ -1206,10 +1206,10 @@
         <v>49</v>
       </c>
       <c r="B12" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>51</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>52</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>3</v>
@@ -1223,10 +1223,10 @@
         <v>50</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>53</v>
+        <v>170</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>3</v>
@@ -1237,13 +1237,13 @@
     </row>
     <row r="14" spans="1:5" ht="285" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>55</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>57</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>3</v>
@@ -1254,13 +1254,13 @@
     </row>
     <row r="15" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="8" t="s">
         <v>65</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>67</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>3</v>
@@ -1271,13 +1271,13 @@
     </row>
     <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>59</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>61</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>3</v>
@@ -1288,13 +1288,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>62</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>64</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>3</v>
@@ -1305,13 +1305,13 @@
     </row>
     <row r="18" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>3</v>
@@ -1322,13 +1322,13 @@
     </row>
     <row r="19" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>3</v>
@@ -1339,13 +1339,13 @@
     </row>
     <row r="20" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>131</v>
+        <v>172</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>3</v>
@@ -1356,13 +1356,13 @@
     </row>
     <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>71</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>73</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>3</v>
@@ -1373,13 +1373,13 @@
     </row>
     <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>74</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>76</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>3</v>
@@ -1390,13 +1390,13 @@
     </row>
     <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>77</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>79</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>3</v>
@@ -1404,13 +1404,13 @@
     </row>
     <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C24" s="8" t="s">
         <v>78</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>80</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>3</v>
@@ -1418,13 +1418,13 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C25" s="8" t="s">
         <v>81</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>83</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>3</v>
@@ -1432,13 +1432,13 @@
     </row>
     <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>3</v>
@@ -1446,13 +1446,13 @@
     </row>
     <row r="27" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C27" s="8" t="s">
         <v>89</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>91</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>3</v>
@@ -1460,13 +1460,13 @@
     </row>
     <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>3</v>
@@ -1474,13 +1474,13 @@
     </row>
     <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B29" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C29" s="8" t="s">
         <v>86</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>88</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>3</v>
@@ -1488,13 +1488,13 @@
     </row>
     <row r="30" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>3</v>
@@ -1502,13 +1502,13 @@
     </row>
     <row r="31" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C31" s="8" t="s">
         <v>110</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>112</v>
       </c>
       <c r="D31" s="8" t="s">
         <v>3</v>
@@ -1516,13 +1516,13 @@
     </row>
     <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C32" s="8" t="s">
         <v>113</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>115</v>
       </c>
       <c r="D32" s="8" t="s">
         <v>3</v>
@@ -1530,13 +1530,13 @@
     </row>
     <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C33" s="8" t="s">
         <v>116</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>118</v>
       </c>
       <c r="D33" s="8" t="s">
         <v>3</v>
@@ -1544,13 +1544,13 @@
     </row>
     <row r="34" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C34" s="8" t="s">
         <v>119</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>121</v>
       </c>
       <c r="D34" s="8" t="s">
         <v>3</v>
@@ -1558,13 +1558,13 @@
     </row>
     <row r="35" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D35" s="8" t="s">
         <v>3</v>
@@ -1572,13 +1572,13 @@
     </row>
     <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D36" s="8" t="s">
         <v>3</v>
@@ -1586,13 +1586,13 @@
     </row>
     <row r="37" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D37" s="8" t="s">
         <v>3</v>
@@ -1600,13 +1600,13 @@
     </row>
     <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D38" s="8" t="s">
         <v>3</v>
@@ -1614,13 +1614,13 @@
     </row>
     <row r="39" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C39" s="5" t="s">
         <v>97</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>99</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>3</v>
@@ -1628,13 +1628,13 @@
     </row>
     <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>100</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>102</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>3</v>
@@ -1642,13 +1642,13 @@
     </row>
     <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C41" s="5" t="s">
         <v>103</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>105</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>3</v>
@@ -1656,13 +1656,13 @@
     </row>
     <row r="42" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>3</v>
@@ -1670,13 +1670,13 @@
     </row>
     <row r="43" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>3</v>
@@ -1684,13 +1684,13 @@
     </row>
     <row r="44" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>3</v>
@@ -1698,13 +1698,13 @@
     </row>
     <row r="45" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>3</v>
@@ -1712,13 +1712,13 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>3</v>
@@ -1726,13 +1726,13 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>3</v>
@@ -1740,15 +1740,15 @@
       <c r="E47" s="8"/>
       <c r="F47" s="8"/>
     </row>
-    <row r="48" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="B48" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="C48" s="11" t="s">
         <v>151</v>
-      </c>
-      <c r="C48" s="11" t="s">
-        <v>155</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>3</v>
@@ -1756,13 +1756,13 @@
     </row>
     <row r="49" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>3</v>
@@ -1770,13 +1770,13 @@
     </row>
     <row r="50" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>157</v>
+        <v>171</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Added new ENWIAM scripts
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENWIAM.xlsx
+++ b/src/test/resources/xls/ENWIAM.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="3900"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="183">
   <si>
     <t>TCID</t>
   </si>
@@ -555,6 +555,33 @@
   </si>
   <si>
     <t>OPQA-1870||OPQA-1874||OPQA-2390||OPQA-1768||OPQA-1777</t>
+  </si>
+  <si>
+    <t>ENWIAM00018</t>
+  </si>
+  <si>
+    <t>OPQA-2324</t>
+  </si>
+  <si>
+    <t>Verify that the text displayed in 'Did you know ...' Modal is as per wire frames/Conditional Text and Error Messages.</t>
+  </si>
+  <si>
+    <t>ENWIAM00019</t>
+  </si>
+  <si>
+    <t>opqa-1753||opqa-1748||OPQA-3674</t>
+  </si>
+  <si>
+    <t>Verify that,the system should make the ability to logout a Neon session available to ENW.||Verify that when  user signs out of ENW, system will have referrer URL = endnote||Verify  ENW user who signs out, shall be taken to the ENW landing screen and the ENW &amp; Neon session closed.</t>
+  </si>
+  <si>
+    <t>ENWIAM00020</t>
+  </si>
+  <si>
+    <t>OPQA-1995</t>
+  </si>
+  <si>
+    <t>From Neon, Verify that the system is able to merge Activated STeAM account and New Facebook account</t>
   </si>
 </sst>
 </file>
@@ -754,7 +781,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -789,7 +816,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -998,10 +1025,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51:D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1779,6 +1806,48 @@
         <v>153</v>
       </c>
       <c r="D50" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D53" s="2" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added New script ENWIAM60 and Fixed ENWIAM58
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENWIAM.xlsx
+++ b/src/test/resources/xls/ENWIAM.xlsx
@@ -14,12 +14,12 @@
     <sheet name="ENWIAM005" sheetId="9" r:id="rId5"/>
     <sheet name="ENWIAM016" sheetId="10" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="186">
   <si>
     <t>TCID</t>
   </si>
@@ -582,6 +582,15 @@
   </si>
   <si>
     <t>From Neon, Verify that the system is able to merge Activated STeAM account and New Facebook account</t>
+  </si>
+  <si>
+    <t>ENWIAM60</t>
+  </si>
+  <si>
+    <t>OPQA-2911</t>
+  </si>
+  <si>
+    <t>From ENW,Verify that the system is able to merge Neon Active STeAM account and New Facebook account</t>
   </si>
 </sst>
 </file>
@@ -1025,10 +1034,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F53"/>
+  <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51:D53"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39:D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1639,29 +1648,29 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
+    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B40" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C40" s="5" t="s">
         <v>97</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>100</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>3</v>
@@ -1669,83 +1678,83 @@
     </row>
     <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B42" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C42" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="D41" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
+      <c r="D42" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B43" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C43" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="D42" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
+      <c r="D43" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="B43" s="8" t="s">
+      <c r="B44" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="C43" s="8" t="s">
+      <c r="C44" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="D43" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
+      <c r="D44" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="B44" s="8" t="s">
+      <c r="B45" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="C44" s="10" t="s">
+      <c r="C45" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="D44" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
+      <c r="D45" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B46" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="C46" s="5" t="s">
         <v>154</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>140</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>3</v>
@@ -1753,43 +1762,43 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B48" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C48" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="D47" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E47" s="8"/>
-      <c r="F47" s="8"/>
-    </row>
-    <row r="48" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
+      <c r="D48" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E48" s="8"/>
+      <c r="F48" s="8"/>
+    </row>
+    <row r="49" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B49" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="C48" s="11" t="s">
+      <c r="C49" s="11" t="s">
         <v>151</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="C49" s="11" t="s">
-        <v>150</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>3</v>
@@ -1797,27 +1806,27 @@
     </row>
     <row r="50" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C50" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B51" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C50" s="11" t="s">
+      <c r="C51" s="11" t="s">
         <v>153</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>176</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>3</v>
@@ -1825,13 +1834,13 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>3</v>
@@ -1839,15 +1848,29 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B54" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C54" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="D53" s="2" t="s">
+      <c r="D54" s="2" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed forgot password Script In IAM and ENWIAM Module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENWIAM.xlsx
+++ b/src/test/resources/xls/ENWIAM.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="3900"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="13296" windowHeight="3900"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -184,12 +184,6 @@
     <t>ENWIAM013</t>
   </si>
   <si>
-    <t>OPQA-1934||OPQA-1935||OPQA-1945||OPQA-1946||OPQA-1947||OPQA-1950||OPQA-1951||OPQA-1953||OPQA-1948||OPQA-1954||OPQA-1937</t>
-  </si>
-  <si>
-    <t>Verify that Forgot your password? Link is clickable on NEON Landing page and End note landing page||Verify that the system is navigating to Forgot Password page or not, after clicking on Forgot your password? Link||Verify that Upon initiation, the Neon and ENW reset password workflow shall bring the user to the send email verification page where a verification email can be sent to an email address entered by the user.||Verify that the Neon and ENW reset password workflow shall be able to send a verification email to the user||Verify that Upon clicking the link to reset password in the Neon and ENW reset verification email, the user shall be sent to the password reset page to reset the applicable STeAM user||Verify Password must have at least one special character from !@#$%^*()~`{}[]|||Verify Password must contain at least one number is ALWAYS enforced.||Verify Password must have at least one alphabet character either upper or lower case is ALWAYS enforced.||Verify that the Password minimum length of 8 characters is ALWAYS enforced||Verify Upon completion of establishing a new password, a user who wants to go to ENW shall be presented a confirmation page with an optional link back to ENW Landing page||Verify that As a Neon or ENW user, I want to be able to reset my STeAM Password from the EndNote Web landing page.</t>
-  </si>
-  <si>
     <t>ENWIAM014</t>
   </si>
   <si>
@@ -592,12 +586,18 @@
   <si>
     <t>From ENW,Verify that the system is able to merge Neon Active STeAM account and New Facebook account</t>
   </si>
+  <si>
+    <t>OPQA-1934||OPQA-1935&amp;OPQA-3687||OPQA-4230||OPQA-4229||OPQA-4231||OPQA-4232||OPQA-4636||OPQA-4261||OPQA-4244||OPQA-4264||OPQA-4265||OPQA-4237||OPQA-4239||OPQA-4240||OPQA-4246||OPQA-4248||OPQA-4252</t>
+  </si>
+  <si>
+    <t>Verify that Forgot your password? Link is clickable on NEON Landing page and End note landing page||Verify that the system is navigating to Forgot Password page or not, after clicking on Forgot your password? Link&amp;Verify that,the system should support a ENW password reset workflow with the following configurations||Verify that system should not inform user that entered email is not found.||Verify that user should be able to enter email address in Forgot password page.||Verify that  forget password service should send a forgot password email when the email entered is registered in the system||Verify that the platform password reset service should send a platform forget password email with branding that corresponds with the originating application as per wireframe||Verify that When the password reset token in the email is valid, upon clicking the password reset link in the the platform forget password email, the user shall be taken to the External Password Reset Page||Verify that External Password Reset Page should have a new password field where the user enters their new password.||Verify that when reset Password Token already used user should be taken to sign in screen||Verify that upon successful submission of a password change, The user should receive a password change confirmation email to the user's primary email address with branding that corresponds with the application that the user completed the password change||Verify that the password change confirmation email should reference the fact that credentials are shared across all products.||Verify that when the password reset token in the email is expired or already used, upon clicking the password reset link in the the platform forget password email, the user should be taken to the External Invalid Password Reset Token Page.||Verify that the email address on the External Invalid Password Reset Token Page should be pre-populated with the email address that matches the email that the forgot password email was sent.||Verify that user who clicks the submit button on the the External Invalid Password Reset Token page, should be taken to the target application sign in page.||Verify that when Email address is known from password reset token,error message 'The email address is prepopulated.' should be displayed and email address field should be editable||Verify that when Email address is not known from password reset token,email address field should be blank and user should be able to enter any email address||Verify that error message Please enter a valid email address.should be displayed in red color when user enters email address in wrong format</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -822,7 +822,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -857,7 +856,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1033,24 +1031,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:D39"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="70.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="14.44140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.33203125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="70.6640625" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.33203125" style="2" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.33203125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1067,15 +1065,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="158.4">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>3</v>
@@ -1084,15 +1082,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="57.6">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>3</v>
@@ -1101,15 +1099,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="72">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>3</v>
@@ -1118,7 +1116,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="28.8">
       <c r="A5" s="2" t="s">
         <v>34</v>
       </c>
@@ -1135,7 +1133,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="28.8">
       <c r="A6" s="2" t="s">
         <v>35</v>
       </c>
@@ -1152,7 +1150,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="43.2">
       <c r="A7" s="2" t="s">
         <v>38</v>
       </c>
@@ -1169,7 +1167,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="57.6">
       <c r="A8" s="2" t="s">
         <v>39</v>
       </c>
@@ -1186,7 +1184,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="28.8">
       <c r="A9" s="2" t="s">
         <v>42</v>
       </c>
@@ -1203,7 +1201,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="129.6">
       <c r="A10" s="2" t="s">
         <v>47</v>
       </c>
@@ -1220,15 +1218,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="144">
       <c r="A11" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>3</v>
@@ -1237,12 +1235,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>51</v>
@@ -1254,12 +1252,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>52</v>
@@ -1271,518 +1269,518 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="285" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="201.6">
       <c r="A14" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B14" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="144">
+      <c r="A15" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="B15" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="43.2">
+      <c r="A16" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="165" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="B16" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C15" s="8" t="s">
+      <c r="C16" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="86.4">
+      <c r="A18" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="57.6">
+      <c r="A19" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="C19" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="86.4">
+      <c r="A20" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B20" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="28.8">
+      <c r="A21" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C19" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="B21" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="C20" s="10" t="s">
+      <c r="C21" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="28.8">
+      <c r="A22" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="43.2">
+      <c r="A23" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="28.8">
+      <c r="A24" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="28.8">
+      <c r="A26" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="86.4">
+      <c r="A27" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="43.2">
+      <c r="A28" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="28.8">
+      <c r="A29" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="57.6">
+      <c r="A30" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="43.2">
+      <c r="A31" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="28.8">
+      <c r="A32" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="28.8">
+      <c r="A33" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="28.8">
+      <c r="A34" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="28.8">
+      <c r="A35" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="B28" s="2" t="s">
+      <c r="B35" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="28.8">
+      <c r="A36" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="43.2">
+      <c r="A37" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="28.8">
+      <c r="A38" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="28.8">
+      <c r="A39" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="57.6">
+      <c r="A40" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C28" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B30" s="5" t="s">
+      <c r="C40" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="28.8">
+      <c r="A41" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="28.8">
+      <c r="A42" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="57.6">
+      <c r="A43" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C43" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="C30" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="B34" s="5" t="s">
+      <c r="D43" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="43.2">
+      <c r="A44" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="B44" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="72">
+      <c r="A45" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D34" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="B37" s="5" t="s">
+      <c r="B45" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="86.4">
+      <c r="A46" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="B47" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="D37" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="B38" s="5" t="s">
+      <c r="C47" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C38" s="8" t="s">
+      <c r="B48" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="D38" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="D39" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="C44" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="C45" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
+      <c r="C48" s="2" t="s">
         <v>144</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>146</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>3</v>
@@ -1790,85 +1788,85 @@
       <c r="E48" s="8"/>
       <c r="F48" s="8"/>
     </row>
-    <row r="49" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="43.2">
       <c r="A49" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="43.2">
+      <c r="A50" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B50" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="C50" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="43.2">
+      <c r="A51" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C51" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="C49" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="C50" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="C51" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
+      <c r="C52" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="D52" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="B53" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="D52" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
+      <c r="C53" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="D53" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="B54" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="D53" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
+      <c r="C54" s="2" t="s">
         <v>180</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>182</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>3</v>
@@ -1881,23 +1879,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1917,7 +1915,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="3">
         <v>246</v>
       </c>
@@ -1935,7 +1933,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="3">
         <v>247</v>
       </c>
@@ -1953,7 +1951,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="3">
         <v>248</v>
       </c>
@@ -1973,7 +1971,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="2">
         <v>111</v>
       </c>
@@ -1991,7 +1989,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="2">
         <v>111</v>
       </c>
@@ -2021,22 +2019,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -2056,7 +2054,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
@@ -2076,7 +2074,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
         <v>25</v>
       </c>
@@ -2096,7 +2094,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
         <v>26</v>
       </c>
@@ -2116,7 +2114,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="3" t="s">
         <v>28</v>
       </c>
@@ -2136,7 +2134,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="3" t="s">
         <v>29</v>
       </c>
@@ -2166,16 +2164,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -2189,7 +2187,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="2">
         <v>49</v>
       </c>
@@ -2203,7 +2201,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="2">
         <v>50</v>
       </c>
@@ -2217,7 +2215,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="2">
         <v>51</v>
       </c>
@@ -2237,22 +2235,22 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -2266,7 +2264,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="2">
         <v>49</v>
       </c>
@@ -2280,7 +2278,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="2">
         <v>50</v>
       </c>
@@ -2294,7 +2292,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="2">
         <v>51</v>
       </c>
@@ -2314,20 +2312,20 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -2341,7 +2339,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="2">
         <v>91</v>
       </c>
@@ -2355,7 +2353,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="2">
         <v>92</v>
       </c>
@@ -2369,7 +2367,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="2">
         <v>93</v>
       </c>

</xml_diff>

<commit_message>
Merging Scenarios new scripts
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENWIAM.xlsx
+++ b/src/test/resources/xls/ENWIAM.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="13296" windowHeight="3900"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="3900"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -14,12 +14,12 @@
     <sheet name="ENWIAM005" sheetId="9" r:id="rId5"/>
     <sheet name="ENWIAM016" sheetId="10" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="189">
   <si>
     <t>TCID</t>
   </si>
@@ -441,12 +441,6 @@
     <t>ENWIAM90</t>
   </si>
   <si>
-    <t>OPQA-1849</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ENW side Forward Merge: Facebook-New Steam-Activated </t>
-  </si>
-  <si>
     <t>ENWIAM59</t>
   </si>
   <si>
@@ -592,12 +586,28 @@
   <si>
     <t>Verify that Forgot your password? Link is clickable on NEON Landing page and End note landing page||Verify that the system is navigating to Forgot Password page or not, after clicking on Forgot your password? Link&amp;Verify that,the system should support a ENW password reset workflow with the following configurations||Verify that system should not inform user that entered email is not found.||Verify that user should be able to enter email address in Forgot password page.||Verify that  forget password service should send a forgot password email when the email entered is registered in the system||Verify that the platform password reset service should send a platform forget password email with branding that corresponds with the originating application as per wireframe||Verify that When the password reset token in the email is valid, upon clicking the password reset link in the the platform forget password email, the user shall be taken to the External Password Reset Page||Verify that External Password Reset Page should have a new password field where the user enters their new password.||Verify that when reset Password Token already used user should be taken to sign in screen||Verify that upon successful submission of a password change, The user should receive a password change confirmation email to the user's primary email address with branding that corresponds with the application that the user completed the password change||Verify that the password change confirmation email should reference the fact that credentials are shared across all products.||Verify that when the password reset token in the email is expired or already used, upon clicking the password reset link in the the platform forget password email, the user should be taken to the External Invalid Password Reset Token Page.||Verify that the email address on the External Invalid Password Reset Token Page should be pre-populated with the email address that matches the email that the forgot password email was sent.||Verify that user who clicks the submit button on the the External Invalid Password Reset Token page, should be taken to the target application sign in page.||Verify that when Email address is known from password reset token,error message 'The email address is prepopulated.' should be displayed and email address field should be editable||Verify that when Email address is not known from password reset token,email address field should be blank and user should be able to enter any email address||Verify that error message Please enter a valid email address.should be displayed in red color when user enters email address in wrong format</t>
   </si>
+  <si>
+    <t>ENWIAM091</t>
+  </si>
+  <si>
+    <t>OPQA-2042</t>
+  </si>
+  <si>
+    <t>From Neon, Verify that system is able to merge a New steam account and New Facebook account</t>
+  </si>
+  <si>
+    <t>OPQA-1849 || OPQA-2925</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ENW side Forward Merge: Facebook-New Steam-Activated  
+|| From ENW,Verify that system is able to merge a New steam account and New Facebook account</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -822,6 +832,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -856,6 +867,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1031,24 +1043,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F54"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.33203125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="70.6640625" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.33203125" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.33203125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.109375" style="2"/>
+    <col min="1" max="1" width="14.42578125" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="70.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.28515625" style="2" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1065,15 +1077,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="158.4">
+    <row r="2" spans="1:5" ht="195" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>3</v>
@@ -1082,15 +1094,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="57.6">
+    <row r="3" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>3</v>
@@ -1099,15 +1111,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="72">
+    <row r="4" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>3</v>
@@ -1116,7 +1128,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="28.8">
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>34</v>
       </c>
@@ -1133,7 +1145,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="28.8">
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>35</v>
       </c>
@@ -1150,7 +1162,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="43.2">
+    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>38</v>
       </c>
@@ -1167,7 +1179,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="57.6">
+    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>39</v>
       </c>
@@ -1184,7 +1196,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="28.8">
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>42</v>
       </c>
@@ -1201,7 +1213,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="129.6">
+    <row r="10" spans="1:5" ht="150" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>47</v>
       </c>
@@ -1218,15 +1230,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="144">
+    <row r="11" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>3</v>
@@ -1235,12 +1247,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>51</v>
@@ -1252,12 +1264,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>52</v>
@@ -1269,15 +1281,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="201.6">
+    <row r="14" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>3</v>
@@ -1286,7 +1298,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="144">
+    <row r="15" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>54</v>
       </c>
@@ -1303,7 +1315,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="43.2">
+    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>55</v>
       </c>
@@ -1320,7 +1332,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>58</v>
       </c>
@@ -1337,15 +1349,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="86.4">
+    <row r="18" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>3</v>
@@ -1354,7 +1366,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="57.6">
+    <row r="19" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>64</v>
       </c>
@@ -1371,12 +1383,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="86.4">
+    <row r="20" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>125</v>
@@ -1388,7 +1400,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="28.8">
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>67</v>
       </c>
@@ -1405,7 +1417,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="28.8">
+    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>70</v>
       </c>
@@ -1422,7 +1434,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="43.2">
+    <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>73</v>
       </c>
@@ -1436,7 +1448,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="28.8">
+    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>74</v>
       </c>
@@ -1450,7 +1462,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>77</v>
       </c>
@@ -1464,7 +1476,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="28.8">
+    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>80</v>
       </c>
@@ -1478,7 +1490,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="86.4">
+    <row r="27" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>85</v>
       </c>
@@ -1492,7 +1504,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="43.2">
+    <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>88</v>
       </c>
@@ -1506,7 +1518,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="28.8">
+    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>81</v>
       </c>
@@ -1520,21 +1532,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="57.6">
+    <row r="30" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>83</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="43.2">
+    <row r="31" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>106</v>
       </c>
@@ -1548,7 +1560,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="28.8">
+    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>109</v>
       </c>
@@ -1562,7 +1574,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="28.8">
+    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>112</v>
       </c>
@@ -1576,7 +1588,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="28.8">
+    <row r="34" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>115</v>
       </c>
@@ -1590,7 +1602,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="28.8">
+    <row r="35" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
         <v>127</v>
       </c>
@@ -1604,7 +1616,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="28.8">
+    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>130</v>
       </c>
@@ -1618,7 +1630,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="43.2">
+    <row r="37" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
         <v>133</v>
       </c>
@@ -1632,35 +1644,35 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="28.8">
+    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C38" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="B38" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>141</v>
-      </c>
       <c r="D38" s="8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="28.8">
+    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C39" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="B39" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>183</v>
-      </c>
       <c r="D39" s="8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="57.6">
+    <row r="40" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>93</v>
       </c>
@@ -1674,7 +1686,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="28.8">
+    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>96</v>
       </c>
@@ -1688,7 +1700,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="28.8">
+    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>99</v>
       </c>
@@ -1702,7 +1714,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="57.6">
+    <row r="43" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>102</v>
       </c>
@@ -1710,13 +1722,13 @@
         <v>103</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="43.2">
+    <row r="44" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>118</v>
       </c>
@@ -1730,7 +1742,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="72">
+    <row r="45" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>119</v>
       </c>
@@ -1744,43 +1756,43 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="86.4">
+    <row r="46" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>120</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>136</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>138</v>
+        <v>187</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>188</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>144</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>3</v>
@@ -1788,87 +1800,101 @@
       <c r="E48" s="8"/>
       <c r="F48" s="8"/>
     </row>
-    <row r="49" spans="1:4" ht="43.2">
+    <row r="49" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B50" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="C50" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C51" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C49" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="43.2">
-      <c r="A50" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C50" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="43.2">
-      <c r="A51" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="C51" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52" s="2" t="s">
+      <c r="C52" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="D52" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="B53" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="D52" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="2" t="s">
+      <c r="C53" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="D53" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="B54" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="D53" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="2" t="s">
+      <c r="C54" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="B54" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>180</v>
-      </c>
       <c r="D54" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="D55" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1879,23 +1905,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1915,7 +1941,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>246</v>
       </c>
@@ -1933,7 +1959,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>247</v>
       </c>
@@ -1951,7 +1977,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>248</v>
       </c>
@@ -1971,7 +1997,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>111</v>
       </c>
@@ -1989,7 +2015,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>111</v>
       </c>
@@ -2019,22 +2045,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -2054,7 +2080,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
@@ -2074,7 +2100,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>25</v>
       </c>
@@ -2094,7 +2120,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>26</v>
       </c>
@@ -2114,7 +2140,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>28</v>
       </c>
@@ -2134,7 +2160,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>29</v>
       </c>
@@ -2164,16 +2190,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -2187,7 +2213,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>49</v>
       </c>
@@ -2201,7 +2227,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>50</v>
       </c>
@@ -2215,7 +2241,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>51</v>
       </c>
@@ -2235,22 +2261,22 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -2264,7 +2290,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>49</v>
       </c>
@@ -2278,7 +2304,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>50</v>
       </c>
@@ -2292,7 +2318,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>51</v>
       </c>
@@ -2312,20 +2338,20 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -2339,7 +2365,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>91</v>
       </c>
@@ -2353,7 +2379,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>92</v>
       </c>
@@ -2367,7 +2393,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>93</v>
       </c>

</xml_diff>

<commit_message>
Added few test case numbers to Local.xml
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENWIAM.xlsx
+++ b/src/test/resources/xls/ENWIAM.xlsx
@@ -600,7 +600,7 @@
   </si>
   <si>
     <t xml:space="preserve"> ENW side Forward Merge: Facebook-New Steam-Activated  
-|| From ENW,Verify that system is able to merge a New steam account and New Facebook account</t>
+||From ENW,Verify that system is able to merge a New steam account and New Facebook account</t>
   </si>
 </sst>
 </file>
@@ -708,7 +708,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1046,8 +1046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added new script for ENWIAM
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENWIAM.xlsx
+++ b/src/test/resources/xls/ENWIAM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="192">
   <si>
     <t>TCID</t>
   </si>
@@ -601,6 +601,15 @@
   <si>
     <t xml:space="preserve"> ENW side Forward Merge: Facebook-New Steam-Activated  
 ||From ENW,Verify that system is able to merge a New steam account and New Facebook account</t>
+  </si>
+  <si>
+    <t>ENWIAM081</t>
+  </si>
+  <si>
+    <t>OPQA-2903</t>
+  </si>
+  <si>
+    <t>From ENW,Verify that the system is able to merge New STeAM account and Activated Facebook account and after merge verify STeAM TRUID is changed</t>
   </si>
 </sst>
 </file>
@@ -1044,10 +1053,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F55"/>
+  <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55:D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1895,6 +1904,20 @@
         <v>186</v>
       </c>
       <c r="D55" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="D56" s="2" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New Script : ENWIAM62
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENWIAM.xlsx
+++ b/src/test/resources/xls/ENWIAM.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="3900"/>
@@ -14,12 +14,12 @@
     <sheet name="ENWIAM005" sheetId="9" r:id="rId5"/>
     <sheet name="ENWIAM016" sheetId="10" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="198">
   <si>
     <t>TCID</t>
   </si>
@@ -619,6 +619,15 @@
   </si>
   <si>
     <t>From Neon, Verify that the system is able to merge New STeAM account and Neon Active Facebook account and after merge verify STeAM TRUID is changed</t>
+  </si>
+  <si>
+    <t>ENWIAM62</t>
+  </si>
+  <si>
+    <t>OPQA-2914</t>
+  </si>
+  <si>
+    <t>From ENW,verify that the system is able to merge Activated STeAM account and Neon Active Facebook account and after merge verify STeAM TRUID is changed</t>
   </si>
 </sst>
 </file>
@@ -818,7 +827,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -853,7 +862,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1062,10 +1071,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F57"/>
+  <dimension ref="A1:F58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1888,14 +1897,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>176</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="C54" s="5" t="s">
         <v>178</v>
       </c>
       <c r="D54" s="2" t="s">
@@ -1941,6 +1950,20 @@
         <v>194</v>
       </c>
       <c r="D57" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="D58" s="2" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modified and developed ENW Scripts
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENWIAM.xlsx
+++ b/src/test/resources/xls/ENWIAM.xlsx
@@ -14,12 +14,12 @@
     <sheet name="ENWIAM005" sheetId="9" r:id="rId5"/>
     <sheet name="ENWIAM016" sheetId="10" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="201">
   <si>
     <t>TCID</t>
   </si>
@@ -628,6 +628,15 @@
   </si>
   <si>
     <t>From ENW,verify that the system is able to merge Activated STeAM account and Neon Active Facebook account and after merge verify STeAM TRUID is changed</t>
+  </si>
+  <si>
+    <t>ENWIAM91</t>
+  </si>
+  <si>
+    <t>OPQA-2904</t>
+  </si>
+  <si>
+    <t>From ENW,Verify that the system is able to merge New STeAM account and Neon Active Facebook account and after merge verify STeAM TRUID is changed</t>
   </si>
 </sst>
 </file>
@@ -1071,10 +1080,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F58"/>
+  <dimension ref="A1:F59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1964,6 +1973,20 @@
         <v>197</v>
       </c>
       <c r="D58" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="D59" s="2" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed description in IAM.xlsx and ENWIAM.xlsx file.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENWIAM.xlsx
+++ b/src/test/resources/xls/ENWIAM.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="3900"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="13296" windowHeight="3900"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <sheet name="ENWIAM005" sheetId="9" r:id="rId5"/>
     <sheet name="ENWIAM016" sheetId="10" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -494,9 +494,6 @@
     <t>Verify that email address field should be in standard email ID format .Email address fields should be mandatory.||Verify that,the system should add the non-matching email as an alternate email under the Neon account,after providing correct credentials of an existing STeAM account with a non-matching email address</t>
   </si>
   <si>
-    <t>Verify that ENW registration screen should be displayed and User should be able to enter email address (required), name (required), and password (required).||Verify that "Sign up" link should be displayed on ENW registration page .||Verify that the user should be able click on "sign up" button after filling the above fields correctly.||Verify that user should get an Email verification Link on the registered Email Id .||Verify that after clicking verification link user should get the message as" Success!You have successfully activated your account. Please sign in."||Verify that after completion of verification process,user should be able to sign into ENW ||Verify that after successful registration on the ENW landing screen using Facebook, users who already has Steam account with the same email address are prompted to link their Steam account with the newly created Facebook account.</t>
-  </si>
-  <si>
     <t>OPQA-2007||OPQA-3652||OPQA-2008||OPQA-2009||OPQA-3333</t>
   </si>
   <si>
@@ -638,12 +635,15 @@
   <si>
     <t>From Neon, Verify that user is informed to contact Customer support through an inline error message, when Neon Active STeAM account and  Neon Active Facebook account are attempted to merge. Verify that user is able to see all emails associated with it.</t>
   </si>
+  <si>
+    <t>Verify that ENW registration screen should be displayed and User should be able to enter email address (required), name (required), and password (required).||Verify that "Sign up" link should be displayed on ENW registration page .||Verify that the user should be able click on "sign up" button after filling the above fields correctly.||Verify that user should get an Email activation Link on the registered Email Id .||Verify that after clicking verification link user should get the message as" Success!You have successfully activated your account. Please sign in."||Verify that after completion of verification process,user should be able to sign into ENW ||Verify that after successful registration on the ENW landing screen using Facebook, users who already has Steam account with the same email address are prompted to link their Steam account with the newly created Facebook account.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -836,7 +836,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -868,10 +868,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -903,7 +902,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1079,24 +1077,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="C35" sqref="C34:C35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="70.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="14.44140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.33203125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="70.6640625" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.33203125" style="2" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.33203125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1113,15 +1111,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="158.4">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>154</v>
+        <v>200</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>3</v>
@@ -1130,12 +1128,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="57.6">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>153</v>
@@ -1147,16 +1145,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="72">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>160</v>
-      </c>
       <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
@@ -1164,7 +1162,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="28.8">
       <c r="A5" s="2" t="s">
         <v>34</v>
       </c>
@@ -1181,7 +1179,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="28.8">
       <c r="A6" s="2" t="s">
         <v>35</v>
       </c>
@@ -1198,7 +1196,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="43.2">
       <c r="A7" s="2" t="s">
         <v>38</v>
       </c>
@@ -1215,7 +1213,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="57.6">
       <c r="A8" s="2" t="s">
         <v>39</v>
       </c>
@@ -1232,7 +1230,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="28.8">
       <c r="A9" s="2" t="s">
         <v>42</v>
       </c>
@@ -1249,7 +1247,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="129.6">
       <c r="A10" s="2" t="s">
         <v>47</v>
       </c>
@@ -1266,16 +1264,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="144">
       <c r="A11" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B11" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>156</v>
-      </c>
       <c r="D11" s="4" t="s">
         <v>3</v>
       </c>
@@ -1283,12 +1281,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>51</v>
@@ -1300,12 +1298,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>52</v>
@@ -1317,16 +1315,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="201.6">
       <c r="A14" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B14" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>181</v>
-      </c>
       <c r="D14" s="4" t="s">
         <v>3</v>
       </c>
@@ -1334,7 +1332,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="144">
       <c r="A15" s="2" t="s">
         <v>54</v>
       </c>
@@ -1351,7 +1349,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="43.2">
       <c r="A16" s="2" t="s">
         <v>55</v>
       </c>
@@ -1368,7 +1366,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="2" t="s">
         <v>58</v>
       </c>
@@ -1385,16 +1383,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="86.4">
       <c r="A18" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B18" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>158</v>
-      </c>
       <c r="D18" s="4" t="s">
         <v>3</v>
       </c>
@@ -1402,7 +1400,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="57.6">
       <c r="A19" s="2" t="s">
         <v>64</v>
       </c>
@@ -1419,12 +1417,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="86.4">
       <c r="A20" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>123</v>
@@ -1436,7 +1434,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="28.8">
       <c r="A21" s="2" t="s">
         <v>67</v>
       </c>
@@ -1453,7 +1451,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="28.8">
       <c r="A22" s="2" t="s">
         <v>70</v>
       </c>
@@ -1470,7 +1468,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="43.2">
       <c r="A23" s="4" t="s">
         <v>73</v>
       </c>
@@ -1484,7 +1482,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="28.8">
       <c r="A24" s="4" t="s">
         <v>74</v>
       </c>
@@ -1498,7 +1496,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" s="4" t="s">
         <v>77</v>
       </c>
@@ -1512,7 +1510,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="28.8">
       <c r="A26" s="4" t="s">
         <v>80</v>
       </c>
@@ -1526,7 +1524,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="86.4">
       <c r="A27" s="4" t="s">
         <v>85</v>
       </c>
@@ -1540,7 +1538,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="43.2">
       <c r="A28" s="4" t="s">
         <v>88</v>
       </c>
@@ -1554,7 +1552,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="28.8">
       <c r="A29" s="4" t="s">
         <v>81</v>
       </c>
@@ -1568,7 +1566,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="57.6">
       <c r="A30" s="4" t="s">
         <v>83</v>
       </c>
@@ -1582,21 +1580,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="57.6">
       <c r="A31" s="8" t="s">
         <v>106</v>
       </c>
       <c r="B31" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="C31" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="C31" s="8" t="s">
-        <v>200</v>
-      </c>
       <c r="D31" s="8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="28.8">
       <c r="A32" s="8" t="s">
         <v>107</v>
       </c>
@@ -1610,7 +1608,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="28.8">
       <c r="A33" s="8" t="s">
         <v>110</v>
       </c>
@@ -1624,7 +1622,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="28.8">
       <c r="A34" s="8" t="s">
         <v>113</v>
       </c>
@@ -1638,7 +1636,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="28.8">
       <c r="A35" s="8" t="s">
         <v>125</v>
       </c>
@@ -1652,7 +1650,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="28.8">
       <c r="A36" s="8" t="s">
         <v>128</v>
       </c>
@@ -1666,7 +1664,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="43.2">
       <c r="A37" s="8" t="s">
         <v>131</v>
       </c>
@@ -1680,7 +1678,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="28.8">
       <c r="A38" s="8" t="s">
         <v>135</v>
       </c>
@@ -1694,21 +1692,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="28.8">
       <c r="A39" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="B39" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="C39" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="C39" s="8" t="s">
-        <v>179</v>
-      </c>
       <c r="D39" s="8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="57.6">
       <c r="A40" s="4" t="s">
         <v>93</v>
       </c>
@@ -1722,7 +1720,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="28.8">
       <c r="A41" s="4" t="s">
         <v>96</v>
       </c>
@@ -1736,7 +1734,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="28.8">
       <c r="A42" s="4" t="s">
         <v>99</v>
       </c>
@@ -1750,7 +1748,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="57.6">
       <c r="A43" s="4" t="s">
         <v>102</v>
       </c>
@@ -1764,7 +1762,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="43.2">
       <c r="A44" s="4" t="s">
         <v>116</v>
       </c>
@@ -1778,7 +1776,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="72">
       <c r="A45" s="4" t="s">
         <v>117</v>
       </c>
@@ -1792,7 +1790,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="86.4">
       <c r="A46" s="4" t="s">
         <v>118</v>
       </c>
@@ -1806,21 +1804,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="43.2">
       <c r="A47" s="2" t="s">
         <v>134</v>
       </c>
       <c r="B47" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="C47" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="C47" s="5" t="s">
-        <v>186</v>
-      </c>
       <c r="D47" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6">
       <c r="A48" s="2" t="s">
         <v>138</v>
       </c>
@@ -1836,12 +1834,12 @@
       <c r="E48" s="8"/>
       <c r="F48" s="8"/>
     </row>
-    <row r="49" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="43.2">
       <c r="A49" s="2" t="s">
         <v>141</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C49" s="11" t="s">
         <v>145</v>
@@ -1850,7 +1848,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="43.2">
       <c r="A50" s="2" t="s">
         <v>142</v>
       </c>
@@ -1864,12 +1862,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="43.2">
       <c r="A51" s="2" t="s">
         <v>146</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C51" s="11" t="s">
         <v>147</v>
@@ -1878,113 +1876,113 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4">
       <c r="A52" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="C52" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="D52" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="D52" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
+      <c r="B53" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="C53" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="D53" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="28.8">
+      <c r="A54" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="D53" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
+      <c r="B54" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="C54" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="C54" s="5" t="s">
-        <v>176</v>
-      </c>
       <c r="D54" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" ht="28.8">
       <c r="A55" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B55" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="C55" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="C55" s="5" t="s">
-        <v>184</v>
-      </c>
       <c r="D55" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" ht="28.8">
       <c r="A56" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="C56" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="C56" s="5" t="s">
+      <c r="D56" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="28.8">
+      <c r="A57" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="D56" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
+      <c r="B57" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="C57" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="C57" s="5" t="s">
+      <c r="D57" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="28.8">
+      <c r="A58" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="D57" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
+      <c r="B58" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="C58" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="C58" s="5" t="s">
+      <c r="D58" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="28.8">
+      <c r="A59" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="D58" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
+      <c r="B59" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="C59" s="5" t="s">
         <v>197</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>198</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>3</v>
@@ -1997,23 +1995,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -2033,7 +2031,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="3">
         <v>246</v>
       </c>
@@ -2051,7 +2049,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="3">
         <v>247</v>
       </c>
@@ -2069,7 +2067,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="3">
         <v>248</v>
       </c>
@@ -2089,7 +2087,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="2">
         <v>111</v>
       </c>
@@ -2107,7 +2105,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="2">
         <v>111</v>
       </c>
@@ -2137,22 +2135,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -2172,7 +2170,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
@@ -2192,7 +2190,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
         <v>25</v>
       </c>
@@ -2212,7 +2210,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
         <v>26</v>
       </c>
@@ -2232,7 +2230,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="3" t="s">
         <v>28</v>
       </c>
@@ -2252,7 +2250,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="3" t="s">
         <v>29</v>
       </c>
@@ -2282,16 +2280,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -2305,7 +2303,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="2">
         <v>49</v>
       </c>
@@ -2319,7 +2317,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="2">
         <v>50</v>
       </c>
@@ -2333,7 +2331,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="2">
         <v>51</v>
       </c>
@@ -2353,22 +2351,22 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -2382,7 +2380,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="2">
         <v>49</v>
       </c>
@@ -2396,7 +2394,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="2">
         <v>50</v>
       </c>
@@ -2410,7 +2408,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="2">
         <v>51</v>
       </c>
@@ -2430,20 +2428,20 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -2457,7 +2455,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="2">
         <v>91</v>
       </c>
@@ -2471,7 +2469,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="2">
         <v>92</v>
       </c>
@@ -2485,7 +2483,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="2">
         <v>93</v>
       </c>

</xml_diff>

<commit_message>
Added new forgot password scripts in ENWIAM Module.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENWIAM.xlsx
+++ b/src/test/resources/xls/ENWIAM.xlsx
@@ -633,10 +633,10 @@
     <t>Verify that ENW registration screen should be displayed and User should be able to enter email address (required), name (required), and password (required).||Verify that "Sign up" link should be displayed on ENW registration page .||Verify that the user should be able click on "sign up" button after filling the above fields correctly.||Verify that user should get an Email activation Link on the registered Email Id .||Verify that after clicking verification link user should get the message as" Success!You have successfully activated your account. Please sign in."||Verify that after completion of verification process,user should be able to sign into ENW ||Verify that after successful registration on the ENW landing screen using Facebook, users who already has Steam account with the same email address are prompted to link their Steam account with the newly created Facebook account.</t>
   </si>
   <si>
-    <t>OPQA-1934||OPQA-1935&amp;OPQA-3687||OPQA-4230||OPQA-4229||OPQA-4231||OPQA-4232||OPQA-4636||OPQA-1950||OPQA-1951||OPQA-1953||OPQA-1949||OPQA-4261&amp;&amp;OPQA-1948||OPQA-4244||OPQA-4264||OPQA-4265||OPQA-4237||OPQA-4239||OPQA-4240||OPQA-4246||OPQA-4248||OPQA-4252||OPQA-5399||OPQA-5400</t>
-  </si>
-  <si>
-    <t>Verify that Forgot your password? Link is clickable on NEON Landing page and End note landing page||Verify that the system is navigating to Forgot Password page or not, after clicking on Forgot your password? Link&amp;Verify that,the system should support a ENW password reset workflow with the following configurations||Verify that system should not inform user that entered email is not found.||Verify that user should be able to enter email address in Forgot password page.||Verify that  forget password service should send a forgot password email when the email entered is registered in the system||Verify that the platform password reset service should send a platform forget password email with branding that corresponds with the originating application as per wireframe||Verify that When the password reset token in the email is valid, upon clicking the password reset link in the the platform forget password email, the user shall be taken to the External Password Reset Page||Verify Password must have at least one special character from !@#$%^*()~`{}[]| in reset password page||Verify  Password must contain at least one number is ALWAYS enforced in password reset page||Verify Password must have at least one alphabet character either upper or lower case is ALWAYS enforced in reset password page.||Verify Password Maximum Length of 95 characters is ALWAYS enforced in reset password page.||Verify that External Password Reset Page should have a new password field where the user enters their new password.&amp;&amp;Verify that the Password minimum length of 8 characters is ALWAYS enforced in reset password page.||Verify that when reset Password Token already used user should be taken to sign in screen||Verify that upon successful submission of a password change, The user should receive a password change confirmation email to the user's primary email address with branding that corresponds with the application that the user completed the password change||Verify that the password change confirmation email should reference the fact that credentials are shared across all products.||Verify that when the password reset token in the email is expired or already used, upon clicking the password reset link in the the platform forget password email, the user should be taken to the External Invalid Password Reset Token Page.||Verify that the email address on the External Invalid Password Reset Token Page should be pre-populated with the email address that matches the email that the forgot password email was sent.||Verify that user who clicks the submit button on the the External Invalid Password Reset Token page, should be taken to the target application sign in page.||Verify that when Email address is known from password reset token,error message 'The email address is prepopulated.' should be displayed and email address field should be editable||Verify that when Email address is not known from password reset token,email address field should be blank and user should be able to enter any email address||Verify that error message Please enter a valid email address.should be displayed in red color when user enters email address in wrong format||Verify that error message New password should not match current password. when enter Old and New password are same in reset password page.||Verify that error message New password should not match previous 4 passwords. when enter new password match with previous four passwords in reset password page.</t>
+    <t>OPQA-1934||OPQA-5209||OPQA-5210||OPQA-1935&amp;OPQA-3687||OPQA-4230||OPQA-4229||OPQA-4231||OPQA-4232||OPQA-4636||OPQA-5136&amp;&amp;OPQA-5135||OPQA-1950||OPQA-1951||OPQA-1953||OPQA-1949||OPQA-4261&amp;&amp;OPQA-1948||OPQA-4244||OPQA-4264||OPQA-4265||OPQA-4237||OPQA-4239||OPQA-4240||OPQA-4246||OPQA-4248||OPQA-4252||OPQA-5399||OPQA-5400</t>
+  </si>
+  <si>
+    <t>Verify that Forgot your password? Link is clickable on NEON Landing page and End note landing page||Verify that Thomson Reuters is replaced with Clarivate Analytics to all endnote pages related  forgot password||Verify that the Endnote should be displayed on the forgot password page||Verify that the system is navigating to Forgot Password page or not, after clicking on Forgot your password? Link&amp;Verify that,the system should support a ENW password reset workflow with the following configurations||Verify that system should not inform user that entered email is not found.||Verify that user should be able to enter email address in Forgot password page.||Verify that  forget password service should send a forgot password email when the email entered is registered in the system||Verify that the platform password reset service should send a platform forget password email with branding that corresponds with the originating application as per wireframe||Verify that When the password reset token in the email is valid, upon clicking the password reset link in the the platform forget password email, the user shall be taken to the External Password Reset Page||Verify that 'EndNote' should be moved within the white area and should be above 'Forgot Password' text and center aligned&amp;&amp;Verify that Thomson Reuters logo is replaced with Clarivate Analytics logo.||Verify Password must have at least one special character from !@#$%^*()~`{}[]| in reset password page||Verify  Password must contain at least one number is ALWAYS enforced in password reset page||Verify Password must have at least one alphabet character either upper or lower case is ALWAYS enforced in reset password page.||Verify Password Maximum Length of 95 characters is ALWAYS enforced in reset password page.||Verify that External Password Reset Page should have a new password field where the user enters their new password.&amp;&amp;Verify that the Password minimum length of 8 characters is ALWAYS enforced in reset password page.||Verify that when reset Password Token already used user should be taken to sign in screen||Verify that upon successful submission of a password change, The user should receive a password change confirmation email to the user's primary email address with branding that corresponds with the application that the user completed the password change||Verify that the password change confirmation email should reference the fact that credentials are shared across all products.||Verify that when the password reset token in the email is expired or already used, upon clicking the password reset link in the the platform forget password email, the user should be taken to the External Invalid Password Reset Token Page.||Verify that the email address on the External Invalid Password Reset Token Page should be pre-populated with the email address that matches the email that the forgot password email was sent.||Verify that user who clicks the submit button on the the External Invalid Password Reset Token page, should be taken to the target application sign in page.||Verify that when Email address is known from password reset token,error message 'The email address is prepopulated.' should be displayed and email address field should be editable||Verify that when Email address is not known from password reset token,email address field should be blank and user should be able to enter any email address||Verify that error message Please enter a valid email address.should be displayed in red color when user enters email address in wrong format||Verify that error message New password should not match current password. when enter Old and New password are same in reset password page.||Verify that error message New password should not match previous 4 passwords. when enter new password match with previous four passwords in reset password page.</t>
   </si>
 </sst>
 </file>
@@ -1315,7 +1315,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="201.6">
+    <row r="14" spans="1:5" ht="216">
       <c r="A14" s="2" t="s">
         <v>53</v>
       </c>

</xml_diff>

<commit_message>
Modified Scripts in IAM Module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENWIAM.xlsx
+++ b/src/test/resources/xls/ENWIAM.xlsx
@@ -633,10 +633,10 @@
     <t>Verify that ENW registration screen should be displayed and User should be able to enter email address (required), name (required), and password (required).||Verify that "Sign up" link should be displayed on ENW registration page .||Verify that the user should be able click on "sign up" button after filling the above fields correctly.||Verify that user should get an Email activation Link on the registered Email Id .||Verify that after clicking verification link user should get the message as" Success!You have successfully activated your account. Please sign in."||Verify that after completion of verification process,user should be able to sign into ENW ||Verify that after successful registration on the ENW landing screen using Facebook, users who already has Steam account with the same email address are prompted to link their Steam account with the newly created Facebook account.</t>
   </si>
   <si>
-    <t>OPQA-1934||OPQA-5209||OPQA-5210||OPQA-1935&amp;OPQA-3687||OPQA-4230||OPQA-4229||OPQA-4231||OPQA-4232||OPQA-4636||OPQA-5136&amp;&amp;OPQA-5135||OPQA-1950||OPQA-1951||OPQA-1953||OPQA-1949||OPQA-4261&amp;&amp;OPQA-1948||OPQA-4244||OPQA-4264||OPQA-4265||OPQA-4237||OPQA-4239||OPQA-4240||OPQA-4246||OPQA-4248||OPQA-4252||OPQA-5399||OPQA-5400</t>
-  </si>
-  <si>
-    <t>Verify that Forgot your password? Link is clickable on NEON Landing page and End note landing page||Verify that Thomson Reuters is replaced with Clarivate Analytics to all endnote pages related  forgot password||Verify that the Endnote should be displayed on the forgot password page||Verify that the system is navigating to Forgot Password page or not, after clicking on Forgot your password? Link&amp;Verify that,the system should support a ENW password reset workflow with the following configurations||Verify that system should not inform user that entered email is not found.||Verify that user should be able to enter email address in Forgot password page.||Verify that  forget password service should send a forgot password email when the email entered is registered in the system||Verify that the platform password reset service should send a platform forget password email with branding that corresponds with the originating application as per wireframe||Verify that When the password reset token in the email is valid, upon clicking the password reset link in the the platform forget password email, the user shall be taken to the External Password Reset Page||Verify that 'EndNote' should be moved within the white area and should be above 'Forgot Password' text and center aligned&amp;&amp;Verify that Thomson Reuters logo is replaced with Clarivate Analytics logo.||Verify Password must have at least one special character from !@#$%^*()~`{}[]| in reset password page||Verify  Password must contain at least one number is ALWAYS enforced in password reset page||Verify Password must have at least one alphabet character either upper or lower case is ALWAYS enforced in reset password page.||Verify Password Maximum Length of 95 characters is ALWAYS enforced in reset password page.||Verify that External Password Reset Page should have a new password field where the user enters their new password.&amp;&amp;Verify that the Password minimum length of 8 characters is ALWAYS enforced in reset password page.||Verify that when reset Password Token already used user should be taken to sign in screen||Verify that upon successful submission of a password change, The user should receive a password change confirmation email to the user's primary email address with branding that corresponds with the application that the user completed the password change||Verify that the password change confirmation email should reference the fact that credentials are shared across all products.||Verify that when the password reset token in the email is expired or already used, upon clicking the password reset link in the the platform forget password email, the user should be taken to the External Invalid Password Reset Token Page.||Verify that the email address on the External Invalid Password Reset Token Page should be pre-populated with the email address that matches the email that the forgot password email was sent.||Verify that user who clicks the submit button on the the External Invalid Password Reset Token page, should be taken to the target application sign in page.||Verify that when Email address is known from password reset token,error message 'The email address is prepopulated.' should be displayed and email address field should be editable||Verify that when Email address is not known from password reset token,email address field should be blank and user should be able to enter any email address||Verify that error message Please enter a valid email address.should be displayed in red color when user enters email address in wrong format||Verify that error message New password should not match current password. when enter Old and New password are same in reset password page.||Verify that error message New password should not match previous 4 passwords. when enter new password match with previous four passwords in reset password page.</t>
+    <t>OPQA-1934||OPQA-5209&amp;&amp;OPQA-5135||OPQA-5210&amp;&amp;OPQA-5136||OPQA-1935&amp;OPQA-3687||OPQA-4230||OPQA-4229||OPQA-4231||OPQA-4232||OPQA-4636||OPQA-5130&amp;&amp;OPQA-5129||OPQA-1950||OPQA-1951||OPQA-1953||OPQA-1949||OPQA-4261&amp;&amp;OPQA-1948||OPQA-4244||OPQA-4264||OPQA-4265||OPQA-4237||OPQA-4239||OPQA-4240||OPQA-4246||OPQA-4248||OPQA-4252||OPQA-5399||OPQA-5400</t>
+  </si>
+  <si>
+    <t>Verify that Forgot your password? Link is clickable on NEON Landing page and End note landing page||Verify that Thomson Reuters is replaced with Clarivate Analytics to all endnote pages related  forgot password&amp;&amp;Verify that Thomson Reuters logo is replaced with Clarivate Analytics logo. and placed below the white area||Verify that the Endnote should be displayed on the forgot password page&amp;&amp;Verify that 'EndNote' should be moved within the white area and should be above 'Forgot Password' text and center aligned||Verify that the system is navigating to Forgot Password page or not, after clicking on Forgot your password? Link&amp;Verify that,the system should support a ENW password reset workflow with the following configurations||Verify that system should not inform user that entered email is not found.||Verify that user should be able to enter email address in Forgot password page.||Verify that  forget password service should send a forgot password email when the email entered is registered in the system||Verify that the platform password reset service should send a platform forget password email with branding that corresponds with the originating application as per wireframe||Verify that When the password reset token in the email is valid, upon clicking the password reset link in the the platform forget password email, the user shall be taken to the External Password Reset Page||Verify that 'EndNote' should be moved within the white area and should be above 'Reset your Password' text and center aligned&amp;&amp;Verify that Thomson Reuters logo is replaced with Clarivate Analytics logo.||Verify Password must have at least one special character from !@#$%^*()~`{}[]| in reset password page||Verify  Password must contain at least one number is ALWAYS enforced in password reset page||Verify Password must have at least one alphabet character either upper or lower case is ALWAYS enforced in reset password page.||Verify Password Maximum Length of 95 characters is ALWAYS enforced in reset password page.||Verify that External Password Reset Page should have a new password field where the user enters their new password.&amp;&amp;Verify that the Password minimum length of 8 characters is ALWAYS enforced in reset password page.||Verify that when reset Password Token already used user should be taken to sign in screen||Verify that upon successful submission of a password change, The user should receive a password change confirmation email to the user's primary email address with branding that corresponds with the application that the user completed the password change||Verify that the password change confirmation email should reference the fact that credentials are shared across all products.||Verify that when the password reset token in the email is expired or already used, upon clicking the password reset link in the the platform forget password email, the user should be taken to the External Invalid Password Reset Token Page.||Verify that the email address on the External Invalid Password Reset Token Page should be pre-populated with the email address that matches the email that the forgot password email was sent.||Verify that user who clicks the submit button on the the External Invalid Password Reset Token page, should be taken to the target application sign in page.||Verify that when Email address is known from password reset token,error message 'The email address is prepopulated.' should be displayed and email address field should be editable||Verify that when Email address is not known from password reset token,email address field should be blank and user should be able to enter any email address||Verify that error message Please enter a valid email address.should be displayed in red color when user enters email address in wrong format||Verify that error message New password should not match current password. when enter Old and New password are same in reset password page.||Verify that error message New password should not match previous 4 passwords. when enter new password match with previous four passwords in reset password page.</t>
   </si>
 </sst>
 </file>
@@ -1315,7 +1315,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="216">
+    <row r="14" spans="1:5" ht="230.4">
       <c r="A14" s="2" t="s">
         <v>53</v>
       </c>

</xml_diff>

<commit_message>
added testcases to excel
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENWIAM.xlsx
+++ b/src/test/resources/xls/ENWIAM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="13296" windowHeight="3900"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="3900"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <sheet name="ENWIAM005" sheetId="9" r:id="rId5"/>
     <sheet name="ENWIAM016" sheetId="10" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -272,13 +272,7 @@
     <t>ENWIAM50</t>
   </si>
   <si>
-    <t>OPQA-1707||OPQA-1734</t>
-  </si>
-  <si>
     <t>ENWIAM51</t>
-  </si>
-  <si>
-    <t>Verify that Neon Landing page, displays Neon branding , marketing copy , New icon and also integration with Endnote</t>
   </si>
   <si>
     <t>ENWIAM42</t>
@@ -479,12 +473,6 @@
   </si>
   <si>
     <t>OPQA-1848||OPQA-2391</t>
-  </si>
-  <si>
-    <t>OPQA-1673 || OPQA-1681 || OPQA-1691 || OPQA-1817 || OPQA-3648 || OPQA-3649||OPQA-3331</t>
-  </si>
-  <si>
-    <t>Verify that on ENW landing page displays,EndNote branding and marketing copy and integration with Project Neon||Verify that user is able to see login through Shibboleth link in ENW Login screen and upon clicking the link it should navigate to proper URL to Login</t>
   </si>
   <si>
     <t>Verify that [X] and "not now" button is working while linking two social accounts.
@@ -637,6 +625,18 @@
   </si>
   <si>
     <t>Verify that Forgot your password? Link is clickable on NEON Landing page and End note landing page||Verify that Thomson Reuters is replaced with Clarivate Analytics to all endnote pages related  forgot password&amp;&amp;Verify that Thomson Reuters logo is replaced with Clarivate Analytics logo. and placed below the white area||Verify that the Endnote should be displayed on the forgot password page&amp;&amp;Verify that 'EndNote' should be moved within the white area and should be above 'Forgot Password' text and center aligned||Verify that the system is navigating to Forgot Password page or not, after clicking on Forgot your password? Link&amp;Verify that,the system should support a ENW password reset workflow with the following configurations||Verify that system should not inform user that entered email is not found.||Verify that user should be able to enter email address in Forgot password page.||Verify that  forget password service should send a forgot password email when the email entered is registered in the system||Verify that the platform password reset service should send a platform forget password email with branding that corresponds with the originating application as per wireframe||Verify that When the password reset token in the email is valid, upon clicking the password reset link in the the platform forget password email, the user shall be taken to the External Password Reset Page||Verify that 'EndNote' should be moved within the white area and should be above 'Reset your Password' text and center aligned&amp;&amp;Verify that Thomson Reuters logo is replaced with Clarivate Analytics logo.||Verify Password must have at least one special character from !@#$%^*()~`{}[]| in reset password page||Verify  Password must contain at least one number is ALWAYS enforced in password reset page||Verify Password must have at least one alphabet character either upper or lower case is ALWAYS enforced in reset password page.||Verify Password Maximum Length of 95 characters is ALWAYS enforced in reset password page.||Verify that External Password Reset Page should have a new password field where the user enters their new password.&amp;&amp;Verify that the Password minimum length of 8 characters is ALWAYS enforced in reset password page.||Verify that when reset Password Token already used user should be taken to sign in screen||Verify that upon successful submission of a password change, The user should receive a password change confirmation email to the user's primary email address with branding that corresponds with the application that the user completed the password change||Verify that the password change confirmation email should reference the fact that credentials are shared across all products.||Verify that when the password reset token in the email is expired or already used, upon clicking the password reset link in the the platform forget password email, the user should be taken to the External Invalid Password Reset Token Page.||Verify that the email address on the External Invalid Password Reset Token Page should be pre-populated with the email address that matches the email that the forgot password email was sent.||Verify that user who clicks the submit button on the the External Invalid Password Reset Token page, should be taken to the target application sign in page.||Verify that when Email address is known from password reset token,error message 'The email address is prepopulated.' should be displayed and email address field should be editable||Verify that when Email address is not known from password reset token,email address field should be blank and user should be able to enter any email address||Verify that error message Please enter a valid email address.should be displayed in red color when user enters email address in wrong format||Verify that error message New password should not match current password. when enter Old and New password are same in reset password page.||Verify that error message New password should not match previous 4 passwords. when enter new password match with previous four passwords in reset password page.</t>
+  </si>
+  <si>
+    <t>OPQA-1707||OPQA-1734||OPQA-5187||OPQA-5188||OPQA-5337||OPQA-5336||OPQA-5334</t>
+  </si>
+  <si>
+    <t>Verify that Neon Landing page, displays Neon branding , marketing copy , New icon and also integration with Endnote||Verify that Neon Landing page, displays Neon branding , marketing copy , New icon and also integration with Endnote||Verify that the Appname 'Project Neon' within white area(above 'Sign in' text and centered).||Verify that the Clarivate Analytics logo is replaced with Thomson Reuters logo and it is placed below and outside white area.||Verify that Clicking on the Clarivate logo shall open the Clarivate marking site in a second browser window /tab||Verify that when the user clicks on the logo it should navigating to Clarivate marketing site (www.clarivate.com).||Verify that the  platform header background color should be white and  Thomson Reuters logo is changed to Clarivate Analytics logo</t>
+  </si>
+  <si>
+    <t>OPQA-1673 || OPQA-1681 || OPQA-1691 || OPQA-1817 || OPQA-3648 || OPQA-3649||OPQA-3331||OPQA-5180||OPQA-5176</t>
+  </si>
+  <si>
+    <t>Verify that on ENW landing page displays,EndNote branding and marketing copy and integration with Project Neon||Verify that user is able to see login through Shibboleth link in ENW Login screen and upon clicking the link it should navigate to proper URL to Login||Verify that on ENW landing page displays,EndNote branding and marketing copy and integration with Project Neon||Verify that user is able to see login through Shibboleth link in ENW Login screen and upon clicking the link it should navigate to proper URL to Login||Verify that the Appname 'EndNote' within white area(above 'Sign in' text and centered).||Verify that the Clarivate Analytics logo is replaced with Thomson Reuters logo and it is placed below and outside white area.</t>
   </si>
 </sst>
 </file>
@@ -1080,18 +1080,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.33203125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="70.6640625" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.33203125" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.33203125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.109375" style="2"/>
+    <col min="1" max="1" width="14.42578125" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="70.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.28515625" style="2" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1111,15 +1111,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="158.4">
+    <row r="2" spans="1:5" ht="195">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>3</v>
@@ -1128,15 +1128,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="57.6">
+    <row r="3" spans="1:5" ht="75">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>3</v>
@@ -1145,15 +1145,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="72">
+    <row r="4" spans="1:5" ht="75">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>3</v>
@@ -1162,7 +1162,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="28.8">
+    <row r="5" spans="1:5" ht="30">
       <c r="A5" s="2" t="s">
         <v>34</v>
       </c>
@@ -1179,7 +1179,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="28.8">
+    <row r="6" spans="1:5" ht="30">
       <c r="A6" s="2" t="s">
         <v>35</v>
       </c>
@@ -1196,7 +1196,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="43.2">
+    <row r="7" spans="1:5" ht="60">
       <c r="A7" s="2" t="s">
         <v>38</v>
       </c>
@@ -1213,7 +1213,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="57.6">
+    <row r="8" spans="1:5" ht="60">
       <c r="A8" s="2" t="s">
         <v>39</v>
       </c>
@@ -1230,7 +1230,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="28.8">
+    <row r="9" spans="1:5" ht="30">
       <c r="A9" s="2" t="s">
         <v>42</v>
       </c>
@@ -1247,7 +1247,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="129.6">
+    <row r="10" spans="1:5" ht="150">
       <c r="A10" s="2" t="s">
         <v>47</v>
       </c>
@@ -1264,15 +1264,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="144">
+    <row r="11" spans="1:5" ht="165">
       <c r="A11" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>3</v>
@@ -1286,7 +1286,7 @@
         <v>49</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>51</v>
@@ -1303,7 +1303,7 @@
         <v>50</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>52</v>
@@ -1315,15 +1315,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="230.4">
+    <row r="14" spans="1:5" ht="409.5">
       <c r="A14" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>3</v>
@@ -1332,7 +1332,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="144">
+    <row r="15" spans="1:5" ht="165">
       <c r="A15" s="2" t="s">
         <v>54</v>
       </c>
@@ -1349,7 +1349,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="43.2">
+    <row r="16" spans="1:5" ht="45">
       <c r="A16" s="2" t="s">
         <v>55</v>
       </c>
@@ -1383,15 +1383,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="86.4">
+    <row r="18" spans="1:5" ht="90">
       <c r="A18" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>3</v>
@@ -1400,7 +1400,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="57.6">
+    <row r="19" spans="1:5" ht="60">
       <c r="A19" s="2" t="s">
         <v>64</v>
       </c>
@@ -1408,7 +1408,7 @@
         <v>65</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>3</v>
@@ -1417,15 +1417,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="86.4">
+    <row r="20" spans="1:5" ht="90">
       <c r="A20" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>3</v>
@@ -1434,7 +1434,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="28.8">
+    <row r="21" spans="1:5" ht="30">
       <c r="A21" s="2" t="s">
         <v>67</v>
       </c>
@@ -1451,7 +1451,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="28.8">
+    <row r="22" spans="1:5" ht="45">
       <c r="A22" s="2" t="s">
         <v>70</v>
       </c>
@@ -1468,12 +1468,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="43.2">
+    <row r="23" spans="1:5" ht="60">
       <c r="A23" s="4" t="s">
         <v>73</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>75</v>
@@ -1482,12 +1482,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="28.8">
+    <row r="24" spans="1:5" ht="45">
       <c r="A24" s="4" t="s">
         <v>74</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>76</v>
@@ -1510,309 +1510,309 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="28.8">
+    <row r="26" spans="1:5" ht="30">
       <c r="A26" s="4" t="s">
         <v>80</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="90">
+      <c r="A27" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="45">
+      <c r="A28" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C28" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="C26" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="86.4">
-      <c r="A27" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="43.2">
-      <c r="A28" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>91</v>
-      </c>
       <c r="D28" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="28.8">
+    <row r="29" spans="1:5" ht="180">
       <c r="A29" s="4" t="s">
         <v>81</v>
       </c>
       <c r="B29" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="150">
+      <c r="A30" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C29" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="57.6">
-      <c r="A30" s="4" t="s">
-        <v>83</v>
-      </c>
       <c r="B30" s="5" t="s">
-        <v>150</v>
+        <v>199</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>151</v>
+        <v>200</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="57.6">
+    <row r="31" spans="1:5" ht="60">
       <c r="A31" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="30">
+      <c r="A32" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="28.8">
-      <c r="A32" s="8" t="s">
+      <c r="C32" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="D32" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="30">
+      <c r="A33" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="B33" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="D32" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="28.8">
-      <c r="A33" s="8" t="s">
+      <c r="C33" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="D33" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="45">
+      <c r="A34" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="B34" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="D33" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="28.8">
-      <c r="A34" s="8" t="s">
+      <c r="C34" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="D34" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="45">
+      <c r="A35" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="30">
+      <c r="A36" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="45">
+      <c r="A37" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="30">
+      <c r="A38" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="30">
+      <c r="A39" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="60">
+      <c r="A40" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="30">
+      <c r="A41" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="30">
+      <c r="A42" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="60">
+      <c r="A43" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="45">
+      <c r="A44" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="B44" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="75">
+      <c r="A45" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="D34" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="28.8">
-      <c r="A35" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="28.8">
-      <c r="A36" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="43.2">
-      <c r="A37" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="B37" s="5" t="s">
+      <c r="B45" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="90">
+      <c r="A46" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="45">
+      <c r="A47" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="C37" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="28.8">
-      <c r="A38" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="28.8">
-      <c r="A39" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="C39" s="8" t="s">
+      <c r="B47" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="D39" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="57.6">
-      <c r="A40" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="28.8">
-      <c r="A41" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="28.8">
-      <c r="A42" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="57.6">
-      <c r="A43" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="43.2">
-      <c r="A44" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="C44" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="72">
-      <c r="A45" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="C45" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="86.4">
-      <c r="A46" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="43.2">
-      <c r="A47" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>182</v>
-      </c>
       <c r="C47" s="5" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>3</v>
@@ -1820,13 +1820,13 @@
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>138</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>140</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>3</v>
@@ -1834,43 +1834,43 @@
       <c r="E48" s="8"/>
       <c r="F48" s="8"/>
     </row>
-    <row r="49" spans="1:4" ht="43.2">
+    <row r="49" spans="1:4" ht="60">
       <c r="A49" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="45">
+      <c r="A50" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B50" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B49" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="C49" s="11" t="s">
+      <c r="C50" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="45">
+      <c r="A51" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C51" s="11" t="s">
         <v>145</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="43.2">
-      <c r="A50" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="C50" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="43.2">
-      <c r="A51" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C51" s="11" t="s">
-        <v>147</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>3</v>
@@ -1878,13 +1878,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>3</v>
@@ -1892,97 +1892,97 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="30">
+      <c r="A54" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="C54" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="C53" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="28.8">
-      <c r="A54" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C54" s="5" t="s">
+      <c r="D54" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="30">
+      <c r="A55" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="D54" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="28.8">
-      <c r="A55" s="2" t="s">
-        <v>179</v>
-      </c>
       <c r="B55" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="30">
+      <c r="A56" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C55" s="5" t="s">
+      <c r="B56" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="D55" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="28.8">
-      <c r="A56" s="2" t="s">
+      <c r="C56" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="45">
+      <c r="A57" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="C57" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="C56" s="5" t="s">
+      <c r="D57" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="45">
+      <c r="A58" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="D56" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="28.8">
-      <c r="A57" s="2" t="s">
+      <c r="B58" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="C58" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="C57" s="5" t="s">
+      <c r="D58" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="45">
+      <c r="A59" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="D57" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="28.8">
-      <c r="A58" s="2" t="s">
+      <c r="B59" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="C59" s="5" t="s">
         <v>191</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="28.8">
-      <c r="A59" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>195</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>3</v>
@@ -2002,13 +2002,13 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2142,12 +2142,12 @@
       <selection sqref="A1:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2287,7 +2287,7 @@
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
@@ -2358,12 +2358,12 @@
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2435,10 +2435,10 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">

</xml_diff>

<commit_message>
moved iam032/033 to enwiam
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENWIAM.xlsx
+++ b/src/test/resources/xls/ENWIAM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="201">
   <si>
     <t>TCID</t>
   </si>
@@ -619,6 +619,29 @@
   </si>
   <si>
     <t>Verify that on ENW landing page displays,EndNote branding and marketing copy and integration with Project Neon||Verify that user is able to see login through Shibboleth link in ENW Login screen and upon clicking the link it should navigate to proper URL to Login||Verify that on ENW landing page displays,EndNote branding and marketing copy and integration with Project Neon||Verify that user is able to see login through Shibboleth link in ENW Login screen and upon clicking the link it should navigate to proper URL to Login||Verify that the Appname 'EndNote' within white area(above 'Sign in' text and centered).||Verify that the Clarivate Analytics logo is replaced with Thomson Reuters logo and it is placed below and outside white area.</t>
+  </si>
+  <si>
+    <t>OPQA-3879||OPQA-3881||OPQA-3882||OPQA-3883||OPQA-3884||OPQA-3630||OPQA-3631||OPQA-1675</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Sign-in with Steam and link existing social account with matching email.
+2) Sign-in with Steam account which already has linked social account.
+Verify that user should never be prompted to link accounts, when sign in first time on Neon landing screen using social.||Verify that user should be prompted to link accounts, when sign in first time on Neon landing screen using STeAM. (Note:User should already been sign into social)
+</t>
+  </si>
+  <si>
+    <t>OPQA-2119||OPQA-2287||OPQA-2293||OPQA-2305||OPQA-2308||OPQA-2319||OPQA-2336||OPQA-2273||OPQA-3608||OPQA-1825||OPQA-1827||OPQA-1829</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Sign-in with Social and link existing steam  account with matching email.
+2) Sign-in with Social account which already has linked Staem account.
+</t>
+  </si>
+  <si>
+    <t>ENWIAM63</t>
+  </si>
+  <si>
+    <t>ENWIAM64</t>
   </si>
 </sst>
 </file>
@@ -1062,10 +1085,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F57"/>
+  <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1812,7 +1835,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>139</v>
       </c>
@@ -1826,7 +1849,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>157</v>
       </c>
@@ -1840,7 +1863,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>160</v>
       </c>
@@ -1854,7 +1877,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>163</v>
       </c>
@@ -1868,7 +1891,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>169</v>
       </c>
@@ -1882,7 +1905,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>174</v>
       </c>
@@ -1896,7 +1919,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>177</v>
       </c>
@@ -1910,7 +1933,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>180</v>
       </c>
@@ -1924,17 +1947,47 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E57" s="2"/>
+    </row>
+    <row r="58" spans="1:5" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E58" s="2"/>
+    </row>
+    <row r="59" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B59" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="C57" s="5" t="s">
+      <c r="C59" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="D57" s="2" t="s">
+      <c r="D59" s="2" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed script in enwiam module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENWIAM.xlsx
+++ b/src/test/resources/xls/ENWIAM.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="3900"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="13296" windowHeight="3900" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -105,9 +105,6 @@
     <t>Good</t>
   </si>
   <si>
-    <t>Neon@</t>
-  </si>
-  <si>
     <t>Neon@123</t>
   </si>
   <si>
@@ -642,12 +639,15 @@
   <si>
     <t>ENWIAM006</t>
   </si>
+  <si>
+    <t>Neon@1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -840,7 +840,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -872,10 +872,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -907,7 +906,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1083,24 +1081,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+    <sheetView topLeftCell="A36" workbookViewId="0">
       <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="70.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="14.44140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.33203125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="70.6640625" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.33203125" style="2" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.33203125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1117,15 +1115,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="158.4">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>3</v>
@@ -1134,15 +1132,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="57.6">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>3</v>
@@ -1151,16 +1149,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="72">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>147</v>
-      </c>
       <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
@@ -1168,640 +1166,640 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="28.8">
       <c r="A5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="28.8">
+      <c r="A6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="9" t="s">
+      <c r="B6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="D6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="43.2">
+      <c r="A7" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="57.6">
+      <c r="A8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>198</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="B8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="D8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="28.8">
+      <c r="A9" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="B9" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="C9" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="D9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="129.6">
+      <c r="A10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="150" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="C10" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="144">
+      <c r="A11" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="165" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="B11" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="C11" s="8" t="s">
+      <c r="B12" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="230.4">
+      <c r="A14" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="144">
+      <c r="A15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="43.2">
+      <c r="A16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="86.4">
+      <c r="A18" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>186</v>
-      </c>
-      <c r="C14" s="8" t="s">
+      <c r="C18" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="57.6">
+      <c r="A19" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="28.8">
+      <c r="A20" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="28.8">
+      <c r="A21" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="43.2">
+      <c r="A22" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="28.8">
+      <c r="A23" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="28.8">
+      <c r="A25" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="86.4">
+      <c r="A26" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="43.2">
+      <c r="A27" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="158.4">
+      <c r="A28" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="165" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C19" s="8" t="s">
+      <c r="C28" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="144">
+      <c r="A29" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="57.6">
+      <c r="A30" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="28.8">
+      <c r="A31" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="28.8">
+      <c r="A32" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="28.8">
+      <c r="A33" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="28.8">
+      <c r="A34" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="28.8">
+      <c r="A35" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="43.2">
+      <c r="A36" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="28.8">
+      <c r="A37" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="28.8">
+      <c r="A38" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="57.6">
+      <c r="A39" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="28.8">
+      <c r="A40" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="28.8">
+      <c r="A41" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="43.2">
+      <c r="A42" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="72">
+      <c r="A43" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C43" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="180" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="150" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="C36" s="8" t="s">
+      <c r="D43" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="86.4">
+      <c r="A44" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="43.2">
+      <c r="A45" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="D36" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="C37" s="8" t="s">
+      <c r="B45" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D37" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="C43" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
+      <c r="B46" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="C46" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>131</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>3</v>
@@ -1809,185 +1807,185 @@
       <c r="E46" s="8"/>
       <c r="F46" s="8"/>
     </row>
-    <row r="47" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="43.2">
       <c r="A47" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C47" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="43.2">
+      <c r="A48" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B48" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C48" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="43.2">
+      <c r="A49" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C47" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C48" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="C49" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
+      <c r="B50" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="C50" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="D50" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="D50" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
+      <c r="B51" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="C51" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="D51" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="28.8">
+      <c r="A52" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="D51" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
+      <c r="B52" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="C52" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="C52" s="5" t="s">
-        <v>162</v>
-      </c>
       <c r="D52" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" ht="28.8">
       <c r="A53" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="C53" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="C53" s="5" t="s">
-        <v>168</v>
-      </c>
       <c r="D53" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" ht="28.8">
       <c r="A54" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="C54" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="C54" s="5" t="s">
+      <c r="D54" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="28.8">
+      <c r="A55" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="D54" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
+      <c r="B55" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="C55" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="C55" s="5" t="s">
+      <c r="D55" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="28.8">
+      <c r="A56" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="D55" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
+      <c r="B56" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="C56" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="C56" s="5" t="s">
+      <c r="D56" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" customFormat="1" ht="100.8">
+      <c r="A57" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E57" s="2"/>
+    </row>
+    <row r="58" spans="1:5" customFormat="1" ht="100.8">
+      <c r="A58" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E58" s="2"/>
+    </row>
+    <row r="59" spans="1:5" ht="28.8">
+      <c r="A59" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="D56" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E57" s="2"/>
-    </row>
-    <row r="58" spans="1:5" customFormat="1" ht="165" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E58" s="2"/>
-    </row>
-    <row r="59" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
+      <c r="B59" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="C59" s="5" t="s">
         <v>181</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>182</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>3</v>
@@ -2000,23 +1998,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -2036,7 +2034,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="3">
         <v>246</v>
       </c>
@@ -2054,7 +2052,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="3">
         <v>247</v>
       </c>
@@ -2072,7 +2070,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="3">
         <v>248</v>
       </c>
@@ -2092,7 +2090,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="2">
         <v>111</v>
       </c>
@@ -2110,7 +2108,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="2">
         <v>111</v>
       </c>
@@ -2140,22 +2138,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -2175,7 +2173,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
@@ -2195,7 +2193,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
         <v>25</v>
       </c>
@@ -2215,7 +2213,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
         <v>26</v>
       </c>
@@ -2235,9 +2233,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="3" t="s">
-        <v>28</v>
+        <v>200</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>27</v>
@@ -2255,12 +2253,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="C6" s="2">
         <v>5</v>
@@ -2285,16 +2283,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -2308,7 +2306,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="2">
         <v>49</v>
       </c>
@@ -2322,7 +2320,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="2">
         <v>50</v>
       </c>
@@ -2336,7 +2334,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="2">
         <v>51</v>
       </c>
@@ -2356,22 +2354,22 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -2385,7 +2383,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="2">
         <v>49</v>
       </c>
@@ -2399,7 +2397,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="2">
         <v>50</v>
       </c>
@@ -2413,7 +2411,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="2">
         <v>51</v>
       </c>
@@ -2433,20 +2431,20 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -2460,7 +2458,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="2">
         <v>91</v>
       </c>
@@ -2474,7 +2472,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="2">
         <v>92</v>
       </c>
@@ -2488,7 +2486,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="2">
         <v>93</v>
       </c>

</xml_diff>

<commit_message>
Updated sanity all.xml file and added test scripts for dra and endnote.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENWIAM.xlsx
+++ b/src/test/resources/xls/ENWIAM.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="13296" windowHeight="3900" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14805" windowHeight="2955"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -14,12 +14,13 @@
     <sheet name="ENWIAM005" sheetId="9" r:id="rId5"/>
     <sheet name="ENWIAM016" sheetId="10" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="203">
   <si>
     <t>TCID</t>
   </si>
@@ -642,12 +643,18 @@
   <si>
     <t>Neon@1</t>
   </si>
+  <si>
+    <t>Verify that User is able to sign-into EndNote Web using STeAM.</t>
+  </si>
+  <si>
+    <t>ENWIAM020</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -672,6 +679,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -728,7 +742,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -750,6 +764,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -840,7 +857,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -872,9 +889,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -906,6 +924,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1081,24 +1100,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F59"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="B59" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.33203125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="70.6640625" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.33203125" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.33203125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.109375" style="2"/>
+    <col min="1" max="1" width="14.42578125" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="70.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.28515625" style="2" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1115,7 +1134,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="158.4">
+    <row r="2" spans="1:5" ht="195" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -1132,7 +1151,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="57.6">
+    <row r="3" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
@@ -1149,7 +1168,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="72">
+    <row r="4" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -1166,7 +1185,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="28.8">
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>33</v>
       </c>
@@ -1183,7 +1202,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="28.8">
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>34</v>
       </c>
@@ -1200,7 +1219,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="43.2">
+    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>199</v>
       </c>
@@ -1217,7 +1236,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="57.6">
+    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>35</v>
       </c>
@@ -1234,7 +1253,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="28.8">
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>38</v>
       </c>
@@ -1251,7 +1270,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="129.6">
+    <row r="10" spans="1:5" ht="150" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>43</v>
       </c>
@@ -1268,7 +1287,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="144">
+    <row r="11" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>44</v>
       </c>
@@ -1285,7 +1304,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>45</v>
       </c>
@@ -1302,7 +1321,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>46</v>
       </c>
@@ -1319,7 +1338,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="230.4">
+    <row r="14" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>49</v>
       </c>
@@ -1336,7 +1355,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="144">
+    <row r="15" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>50</v>
       </c>
@@ -1353,7 +1372,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="43.2">
+    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>51</v>
       </c>
@@ -1370,7 +1389,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>54</v>
       </c>
@@ -1387,7 +1406,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="86.4">
+    <row r="18" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>58</v>
       </c>
@@ -1404,7 +1423,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="57.6">
+    <row r="19" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>60</v>
       </c>
@@ -1421,7 +1440,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="28.8">
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>62</v>
       </c>
@@ -1438,7 +1457,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="28.8">
+    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>65</v>
       </c>
@@ -1455,7 +1474,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="43.2">
+    <row r="22" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>68</v>
       </c>
@@ -1469,7 +1488,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="28.8">
+    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>69</v>
       </c>
@@ -1483,7 +1502,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>72</v>
       </c>
@@ -1497,7 +1516,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="28.8">
+    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>75</v>
       </c>
@@ -1511,7 +1530,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="86.4">
+    <row r="26" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>78</v>
       </c>
@@ -1525,7 +1544,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="43.2">
+    <row r="27" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>81</v>
       </c>
@@ -1539,7 +1558,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="158.4">
+    <row r="28" spans="1:5" ht="180" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>76</v>
       </c>
@@ -1553,7 +1572,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="144">
+    <row r="29" spans="1:5" ht="150" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>77</v>
       </c>
@@ -1567,7 +1586,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="57.6">
+    <row r="30" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>97</v>
       </c>
@@ -1581,7 +1600,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="28.8">
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>98</v>
       </c>
@@ -1595,7 +1614,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="28.8">
+    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>101</v>
       </c>
@@ -1609,7 +1628,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="28.8">
+    <row r="33" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>104</v>
       </c>
@@ -1623,7 +1642,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="28.8">
+    <row r="34" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>115</v>
       </c>
@@ -1637,7 +1656,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="28.8">
+    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
         <v>118</v>
       </c>
@@ -1651,7 +1670,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="43.2">
+    <row r="36" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>121</v>
       </c>
@@ -1665,7 +1684,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="28.8">
+    <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
         <v>125</v>
       </c>
@@ -1679,7 +1698,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="28.8">
+    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
         <v>162</v>
       </c>
@@ -1693,7 +1712,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="57.6">
+    <row r="39" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>86</v>
       </c>
@@ -1707,7 +1726,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="28.8">
+    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>89</v>
       </c>
@@ -1721,7 +1740,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="28.8">
+    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>92</v>
       </c>
@@ -1735,7 +1754,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="43.2">
+    <row r="42" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>107</v>
       </c>
@@ -1749,7 +1768,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="72">
+    <row r="43" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>108</v>
       </c>
@@ -1763,7 +1782,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="86.4">
+    <row r="44" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>109</v>
       </c>
@@ -1777,7 +1796,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="43.2">
+    <row r="45" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>124</v>
       </c>
@@ -1791,7 +1810,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>128</v>
       </c>
@@ -1807,7 +1826,7 @@
       <c r="E46" s="8"/>
       <c r="F46" s="8"/>
     </row>
-    <row r="47" spans="1:6" ht="43.2">
+    <row r="47" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>131</v>
       </c>
@@ -1821,7 +1840,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="43.2">
+    <row r="48" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>132</v>
       </c>
@@ -1835,7 +1854,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="43.2">
+    <row r="49" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>136</v>
       </c>
@@ -1849,7 +1868,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>153</v>
       </c>
@@ -1863,7 +1882,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>156</v>
       </c>
@@ -1877,7 +1896,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="28.8">
+    <row r="52" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>159</v>
       </c>
@@ -1891,7 +1910,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="28.8">
+    <row r="53" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>165</v>
       </c>
@@ -1905,7 +1924,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="28.8">
+    <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>170</v>
       </c>
@@ -1919,7 +1938,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="28.8">
+    <row r="55" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>173</v>
       </c>
@@ -1933,7 +1952,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="28.8">
+    <row r="56" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>176</v>
       </c>
@@ -1947,7 +1966,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:5" customFormat="1" ht="100.8">
+    <row r="57" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>195</v>
       </c>
@@ -1962,7 +1981,7 @@
       </c>
       <c r="E57" s="2"/>
     </row>
-    <row r="58" spans="1:5" customFormat="1" ht="100.8">
+    <row r="58" spans="1:5" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>196</v>
       </c>
@@ -1977,7 +1996,7 @@
       </c>
       <c r="E58" s="2"/>
     </row>
-    <row r="59" spans="1:5" ht="28.8">
+    <row r="59" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>179</v>
       </c>
@@ -1988,6 +2007,20 @@
         <v>181</v>
       </c>
       <c r="D59" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="C60" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="D60" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1998,23 +2031,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -2034,7 +2067,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>246</v>
       </c>
@@ -2052,7 +2085,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>247</v>
       </c>
@@ -2070,7 +2103,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>248</v>
       </c>
@@ -2090,7 +2123,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>111</v>
       </c>
@@ -2108,7 +2141,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>111</v>
       </c>
@@ -2138,22 +2171,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -2173,7 +2206,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
@@ -2193,7 +2226,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>25</v>
       </c>
@@ -2213,7 +2246,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>26</v>
       </c>
@@ -2233,7 +2266,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>200</v>
       </c>
@@ -2253,7 +2286,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>28</v>
       </c>
@@ -2283,16 +2316,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -2306,7 +2339,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>49</v>
       </c>
@@ -2320,7 +2353,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>50</v>
       </c>
@@ -2334,7 +2367,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>51</v>
       </c>
@@ -2354,22 +2387,22 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -2383,7 +2416,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>49</v>
       </c>
@@ -2397,7 +2430,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>50</v>
       </c>
@@ -2411,7 +2444,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>51</v>
       </c>
@@ -2431,20 +2464,20 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -2458,7 +2491,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>91</v>
       </c>
@@ -2472,7 +2505,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>92</v>
       </c>
@@ -2486,7 +2519,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>93</v>
       </c>

</xml_diff>